<commit_message>
Update to writing excel file
</commit_message>
<xml_diff>
--- a/Data/Example_DB.xlsx
+++ b/Data/Example_DB.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jones\Documents\Group1_Project_Middle-Backend\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jones\Documents\Group1_Project_Middle-Backend\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6A65B9C-DD39-4FA0-9FB0-9F57804ABC71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C1D99C3-F091-4B13-AA95-4B92412C2517}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,10 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="51">
-  <si>
-    <t>Name</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
   <si>
     <t>College</t>
   </si>
@@ -117,16 +114,10 @@
     <t>Mode</t>
   </si>
   <si>
-    <t>Location Impact</t>
-  </si>
-  <si>
     <t>Time Commitment</t>
   </si>
   <si>
     <t>Admission Type</t>
-  </si>
-  <si>
-    <t>Test 1</t>
   </si>
   <si>
     <t>Anthropology is Elemental</t>
@@ -191,12 +182,18 @@
   <si>
     <t>{439e710e-9363-46fe-b6b8-d105e96ee7e6}</t>
   </si>
+  <si>
+    <t>Project Name</t>
+  </si>
+  <si>
+    <t>Impact</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -256,6 +253,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="11">
@@ -615,13 +619,13 @@
       <alignment readingOrder="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -629,48 +633,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="35">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFF3F3F3"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FFCCCCCC"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFCCCCCC"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFCCCCCC"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FFCCCCCC"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
+  <dxfs count="34">
     <dxf>
       <font>
         <b val="0"/>
@@ -1960,43 +1923,42 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{021725A4-9911-4075-ACE0-7C275C0682F5}" name="Database" displayName="Database" ref="A1:AD252" totalsRowShown="0" headerRowDxfId="34" dataDxfId="32" headerRowBorderDxfId="33" tableBorderDxfId="31" totalsRowBorderDxfId="30">
-  <autoFilter ref="A1:AD252" xr:uid="{283055BC-6992-46EF-93EC-D63EC49B5B4D}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{021725A4-9911-4075-ACE0-7C275C0682F5}" name="Database" displayName="Database" ref="A1:AC252" totalsRowShown="0" headerRowDxfId="33" dataDxfId="31" headerRowBorderDxfId="32" tableBorderDxfId="30" totalsRowBorderDxfId="29">
+  <autoFilter ref="A1:AC252" xr:uid="{283055BC-6992-46EF-93EC-D63EC49B5B4D}">
     <filterColumn colId="15">
       <filters blank="1"/>
     </filterColumn>
   </autoFilter>
-  <tableColumns count="30">
-    <tableColumn id="1" xr3:uid="{847DB684-452D-474B-B4CF-E2A20A0C3D1B}" name="Name" dataDxfId="29"/>
-    <tableColumn id="2" xr3:uid="{59293F74-7B5E-4F3C-8DD2-AB9F2B403D0B}" name="College" dataDxfId="28"/>
-    <tableColumn id="3" xr3:uid="{08070D1E-593D-4BA9-85BF-DC77AF3AD41E}" name="Department" dataDxfId="27"/>
-    <tableColumn id="4" xr3:uid="{946ACEDE-8BEC-48F7-AF1F-2624C8ABE677}" name="Academic Level" dataDxfId="26"/>
-    <tableColumn id="5" xr3:uid="{69E6FF92-8958-40AE-A304-D8C47B57D3CB}" name="Class Level" dataDxfId="25"/>
-    <tableColumn id="6" xr3:uid="{0BD375E2-3891-4A9C-8F82-A41A72D7BAE1}" name="Course" dataDxfId="24"/>
-    <tableColumn id="7" xr3:uid="{FC7BE243-0269-4D11-ADB6-8F63638E9D25}" name="Section" dataDxfId="23"/>
-    <tableColumn id="8" xr3:uid="{EC150928-3DBA-45AE-8EDF-D1D64112E692}" name="Primary Focus Area" dataDxfId="22"/>
-    <tableColumn id="9" xr3:uid="{68E1B4A1-1CB5-4960-A4B0-17116AAEFA6A}" name="Start Date" dataDxfId="21"/>
-    <tableColumn id="10" xr3:uid="{0E085481-328C-4E65-9322-9AD9265925D3}" name="End Date" dataDxfId="20"/>
-    <tableColumn id="11" xr3:uid="{E4397740-57CA-46FA-8520-62C0E626DD67}" name="Project Description" dataDxfId="19"/>
-    <tableColumn id="12" xr3:uid="{869A981C-880D-469D-B8A3-AAB3597679F1}" name="Semester" dataDxfId="18"/>
-    <tableColumn id="13" xr3:uid="{E7279675-F476-45AB-B894-8E9CCE9941AF}" name="Status" dataDxfId="17"/>
-    <tableColumn id="14" xr3:uid="{D343B0FA-DE0B-48DF-81BE-F5413B882F80}" name="Compensation" dataDxfId="16"/>
-    <tableColumn id="15" xr3:uid="{9B59FBF9-7D8D-4500-9998-967297331C1D}" name="Opportunity Type" dataDxfId="15"/>
-    <tableColumn id="16" xr3:uid="{F32CB9BD-DB6D-4349-8C8A-B00B55F79297}" name="University Partner" dataDxfId="14"/>
-    <tableColumn id="17" xr3:uid="{39DA1768-46DF-419A-BDD4-EEF497F6B08E}" name="Community Partner: Internal/External" dataDxfId="13"/>
-    <tableColumn id="18" xr3:uid="{12D9CAA8-39A1-40D2-884E-EC75048A674E}" name="Community Partner: Organization" dataDxfId="12"/>
-    <tableColumn id="19" xr3:uid="{206A4F6F-235B-499A-A9B8-0D08FD43CE31}" name="Community Partner: Type" dataDxfId="11"/>
-    <tableColumn id="20" xr3:uid="{1E2E0EF8-54B5-47C7-B720-33AF2B39B266}" name="Community Partner: Contact" dataDxfId="10"/>
-    <tableColumn id="21" xr3:uid="{EF718684-BF1E-41FF-A3A0-12785C419D73}" name="Community Partner: Website" dataDxfId="9"/>
-    <tableColumn id="22" xr3:uid="{ED7C0E2E-5C5E-45D2-A743-CAC587598912}" name="Number of Participants" dataDxfId="8"/>
-    <tableColumn id="23" xr3:uid="{52CDB78D-43F0-4182-8A92-4D1087572CC2}" name="City" dataDxfId="7"/>
-    <tableColumn id="24" xr3:uid="{DFBFB6EA-B301-4F5D-ACFF-296220DFCA37}" name="State" dataDxfId="6"/>
-    <tableColumn id="25" xr3:uid="{2B7AAA1D-9C18-4D3B-9D54-35035361AA1E}" name="Country" dataDxfId="5"/>
-    <tableColumn id="26" xr3:uid="{2E8EC4BD-8E1B-4912-9EDE-EEAD290452C2}" name="Mode" dataDxfId="4"/>
-    <tableColumn id="27" xr3:uid="{C54D5F24-9754-4979-A614-16720F85392E}" name="Location Impact" dataDxfId="3"/>
-    <tableColumn id="28" xr3:uid="{DF6F4B4C-F182-4B14-9A3F-79288BEBD82D}" name="Time Commitment" dataDxfId="2"/>
-    <tableColumn id="29" xr3:uid="{CF21ED53-3A53-4886-9650-257096512121}" name="Admission Type" dataDxfId="1"/>
-    <tableColumn id="30" xr3:uid="{4A6DE2F4-537E-4B94-AA72-9A161D4AB0C4}" name="Test 1" dataDxfId="0"/>
+  <tableColumns count="29">
+    <tableColumn id="1" xr3:uid="{847DB684-452D-474B-B4CF-E2A20A0C3D1B}" name="Project Name" dataDxfId="28"/>
+    <tableColumn id="2" xr3:uid="{59293F74-7B5E-4F3C-8DD2-AB9F2B403D0B}" name="College" dataDxfId="27"/>
+    <tableColumn id="3" xr3:uid="{08070D1E-593D-4BA9-85BF-DC77AF3AD41E}" name="Department" dataDxfId="26"/>
+    <tableColumn id="4" xr3:uid="{946ACEDE-8BEC-48F7-AF1F-2624C8ABE677}" name="Academic Level" dataDxfId="25"/>
+    <tableColumn id="5" xr3:uid="{69E6FF92-8958-40AE-A304-D8C47B57D3CB}" name="Class Level" dataDxfId="24"/>
+    <tableColumn id="6" xr3:uid="{0BD375E2-3891-4A9C-8F82-A41A72D7BAE1}" name="Course" dataDxfId="23"/>
+    <tableColumn id="7" xr3:uid="{FC7BE243-0269-4D11-ADB6-8F63638E9D25}" name="Section" dataDxfId="22"/>
+    <tableColumn id="8" xr3:uid="{EC150928-3DBA-45AE-8EDF-D1D64112E692}" name="Primary Focus Area" dataDxfId="21"/>
+    <tableColumn id="9" xr3:uid="{68E1B4A1-1CB5-4960-A4B0-17116AAEFA6A}" name="Start Date" dataDxfId="20"/>
+    <tableColumn id="10" xr3:uid="{0E085481-328C-4E65-9322-9AD9265925D3}" name="End Date" dataDxfId="19"/>
+    <tableColumn id="11" xr3:uid="{E4397740-57CA-46FA-8520-62C0E626DD67}" name="Project Description" dataDxfId="18"/>
+    <tableColumn id="12" xr3:uid="{869A981C-880D-469D-B8A3-AAB3597679F1}" name="Semester" dataDxfId="17"/>
+    <tableColumn id="13" xr3:uid="{E7279675-F476-45AB-B894-8E9CCE9941AF}" name="Status" dataDxfId="16"/>
+    <tableColumn id="14" xr3:uid="{D343B0FA-DE0B-48DF-81BE-F5413B882F80}" name="Compensation" dataDxfId="15"/>
+    <tableColumn id="15" xr3:uid="{9B59FBF9-7D8D-4500-9998-967297331C1D}" name="Opportunity Type" dataDxfId="14"/>
+    <tableColumn id="16" xr3:uid="{F32CB9BD-DB6D-4349-8C8A-B00B55F79297}" name="University Partner" dataDxfId="13"/>
+    <tableColumn id="17" xr3:uid="{39DA1768-46DF-419A-BDD4-EEF497F6B08E}" name="Community Partner: Internal/External" dataDxfId="12"/>
+    <tableColumn id="18" xr3:uid="{12D9CAA8-39A1-40D2-884E-EC75048A674E}" name="Community Partner: Organization" dataDxfId="11"/>
+    <tableColumn id="19" xr3:uid="{206A4F6F-235B-499A-A9B8-0D08FD43CE31}" name="Community Partner: Type" dataDxfId="10"/>
+    <tableColumn id="20" xr3:uid="{1E2E0EF8-54B5-47C7-B720-33AF2B39B266}" name="Community Partner: Contact" dataDxfId="9"/>
+    <tableColumn id="21" xr3:uid="{EF718684-BF1E-41FF-A3A0-12785C419D73}" name="Community Partner: Website" dataDxfId="8"/>
+    <tableColumn id="22" xr3:uid="{ED7C0E2E-5C5E-45D2-A743-CAC587598912}" name="Number of Participants" dataDxfId="7"/>
+    <tableColumn id="23" xr3:uid="{52CDB78D-43F0-4182-8A92-4D1087572CC2}" name="City" dataDxfId="6"/>
+    <tableColumn id="24" xr3:uid="{DFBFB6EA-B301-4F5D-ACFF-296220DFCA37}" name="State" dataDxfId="5"/>
+    <tableColumn id="25" xr3:uid="{2B7AAA1D-9C18-4D3B-9D54-35035361AA1E}" name="Country" dataDxfId="4"/>
+    <tableColumn id="26" xr3:uid="{2E8EC4BD-8E1B-4912-9EDE-EEAD290452C2}" name="Mode" dataDxfId="3"/>
+    <tableColumn id="27" xr3:uid="{C54D5F24-9754-4979-A614-16720F85392E}" name="Impact" dataDxfId="2"/>
+    <tableColumn id="28" xr3:uid="{DF6F4B4C-F182-4B14-9A3F-79288BEBD82D}" name="Time Commitment" dataDxfId="1"/>
+    <tableColumn id="29" xr3:uid="{CF21ED53-3A53-4886-9650-257096512121}" name="Admission Type" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2299,7 +2261,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AD252"/>
+  <dimension ref="A1:AC252"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
@@ -2336,122 +2298,119 @@
     <col min="29" max="29" width="18.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A1" s="44" t="s">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A1" s="43" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="C1" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="D1" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="45" t="s">
+      <c r="E1" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="27" t="s">
+      <c r="F1" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="27" t="s">
+      <c r="G1" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="27" t="s">
+      <c r="H1" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="27" t="s">
+      <c r="I1" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="27" t="s">
+      <c r="J1" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="27" t="s">
+      <c r="K1" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="32" t="s">
+      <c r="L1" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="27" t="s">
+      <c r="M1" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="27" t="s">
+      <c r="N1" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="27" t="s">
+      <c r="O1" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="27" t="s">
+      <c r="P1" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="27" t="s">
+      <c r="Q1" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="27" t="s">
+      <c r="R1" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="27" t="s">
+      <c r="S1" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="27" t="s">
+      <c r="T1" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="27" t="s">
+      <c r="U1" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="27" t="s">
+      <c r="V1" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="27" t="s">
+      <c r="W1" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="27" t="s">
+      <c r="X1" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="27" t="s">
+      <c r="Y1" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="27" t="s">
+      <c r="Z1" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="27" t="s">
+      <c r="AA1" s="44" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB1" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="27" t="s">
+      <c r="AC1" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="27" t="s">
+    </row>
+    <row r="2" spans="1:29" ht="53.4" x14ac:dyDescent="0.3">
+      <c r="A2" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="28" t="s">
+      <c r="B2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="27" t="s">
+      <c r="C2" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="2" spans="1:30" ht="53.4" x14ac:dyDescent="0.3">
-      <c r="A2" s="20" t="s">
+      <c r="D2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="G2" s="1">
         <v>1</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="I2" s="1">
         <v>2019</v>
@@ -2460,51 +2419,50 @@
         <v>2019</v>
       </c>
       <c r="K2" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="N2" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="O2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="P2" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="R2" s="1"/>
       <c r="S2" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="T2" s="1"/>
       <c r="U2" s="1"/>
       <c r="V2" s="1"/>
       <c r="W2" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="X2" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
       <c r="AA2" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="AB2" s="1"/>
       <c r="AC2" s="25" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
-      <c r="AD2" s="43"/>
-    </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A3" s="21"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -2534,9 +2492,8 @@
       <c r="AA3" s="3"/>
       <c r="AB3" s="3"/>
       <c r="AC3" s="26"/>
-      <c r="AD3" s="3"/>
-    </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A4" s="20"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -2566,9 +2523,8 @@
       <c r="AA4" s="1"/>
       <c r="AB4" s="1"/>
       <c r="AC4" s="25"/>
-      <c r="AD4" s="3"/>
-    </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A5" s="20"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -2598,9 +2554,8 @@
       <c r="AA5" s="1"/>
       <c r="AB5" s="1"/>
       <c r="AC5" s="25"/>
-      <c r="AD5" s="3"/>
-    </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A6" s="21"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -2630,9 +2585,8 @@
       <c r="AA6" s="3"/>
       <c r="AB6" s="3"/>
       <c r="AC6" s="26"/>
-      <c r="AD6" s="3"/>
-    </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A7" s="20"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -2662,9 +2616,8 @@
       <c r="AA7" s="1"/>
       <c r="AB7" s="1"/>
       <c r="AC7" s="25"/>
-      <c r="AD7" s="3"/>
-    </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A8" s="21"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -2694,9 +2647,8 @@
       <c r="AA8" s="3"/>
       <c r="AB8" s="3"/>
       <c r="AC8" s="26"/>
-      <c r="AD8" s="3"/>
-    </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A9" s="21"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -2726,9 +2678,8 @@
       <c r="AA9" s="3"/>
       <c r="AB9" s="3"/>
       <c r="AC9" s="26"/>
-      <c r="AD9" s="3"/>
-    </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A10" s="20"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -2758,9 +2709,8 @@
       <c r="AA10" s="1"/>
       <c r="AB10" s="1"/>
       <c r="AC10" s="25"/>
-      <c r="AD10" s="3"/>
-    </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A11" s="20"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -2790,9 +2740,8 @@
       <c r="AA11" s="1"/>
       <c r="AB11" s="1"/>
       <c r="AC11" s="25"/>
-      <c r="AD11" s="3"/>
-    </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A12" s="21"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -2822,9 +2771,8 @@
       <c r="AA12" s="3"/>
       <c r="AB12" s="3"/>
       <c r="AC12" s="26"/>
-      <c r="AD12" s="3"/>
-    </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A13" s="21"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -2854,9 +2802,8 @@
       <c r="AA13" s="3"/>
       <c r="AB13" s="3"/>
       <c r="AC13" s="26"/>
-      <c r="AD13" s="3"/>
-    </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A14" s="21"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -2886,9 +2833,8 @@
       <c r="AA14" s="3"/>
       <c r="AB14" s="3"/>
       <c r="AC14" s="26"/>
-      <c r="AD14" s="3"/>
-    </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A15" s="21"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -2918,9 +2864,8 @@
       <c r="AA15" s="3"/>
       <c r="AB15" s="3"/>
       <c r="AC15" s="26"/>
-      <c r="AD15" s="3"/>
-    </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A16" s="20"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -2950,9 +2895,8 @@
       <c r="AA16" s="1"/>
       <c r="AB16" s="1"/>
       <c r="AC16" s="25"/>
-      <c r="AD16" s="3"/>
-    </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A17" s="21"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -2982,9 +2926,8 @@
       <c r="AA17" s="3"/>
       <c r="AB17" s="3"/>
       <c r="AC17" s="26"/>
-      <c r="AD17" s="3"/>
-    </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A18" s="20"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -3014,9 +2957,8 @@
       <c r="AA18" s="1"/>
       <c r="AB18" s="1"/>
       <c r="AC18" s="25"/>
-      <c r="AD18" s="3"/>
-    </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A19" s="21"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -3046,9 +2988,8 @@
       <c r="AA19" s="3"/>
       <c r="AB19" s="3"/>
       <c r="AC19" s="26"/>
-      <c r="AD19" s="3"/>
-    </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A20" s="20"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -3078,9 +3019,8 @@
       <c r="AA20" s="1"/>
       <c r="AB20" s="1"/>
       <c r="AC20" s="25"/>
-      <c r="AD20" s="3"/>
-    </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A21" s="20"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -3110,9 +3050,8 @@
       <c r="AA21" s="1"/>
       <c r="AB21" s="1"/>
       <c r="AC21" s="25"/>
-      <c r="AD21" s="3"/>
-    </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A22" s="21"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -3142,9 +3081,8 @@
       <c r="AA22" s="3"/>
       <c r="AB22" s="3"/>
       <c r="AC22" s="26"/>
-      <c r="AD22" s="3"/>
-    </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A23" s="20"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -3174,9 +3112,8 @@
       <c r="AA23" s="1"/>
       <c r="AB23" s="1"/>
       <c r="AC23" s="25"/>
-      <c r="AD23" s="3"/>
-    </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A24" s="21"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -3206,9 +3143,8 @@
       <c r="AA24" s="3"/>
       <c r="AB24" s="3"/>
       <c r="AC24" s="26"/>
-      <c r="AD24" s="3"/>
-    </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A25" s="20"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -3238,9 +3174,8 @@
       <c r="AA25" s="1"/>
       <c r="AB25" s="1"/>
       <c r="AC25" s="25"/>
-      <c r="AD25" s="3"/>
-    </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A26" s="21"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -3270,9 +3205,8 @@
       <c r="AA26" s="3"/>
       <c r="AB26" s="3"/>
       <c r="AC26" s="26"/>
-      <c r="AD26" s="3"/>
-    </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A27" s="21"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -3302,9 +3236,8 @@
       <c r="AA27" s="3"/>
       <c r="AB27" s="3"/>
       <c r="AC27" s="26"/>
-      <c r="AD27" s="3"/>
-    </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A28" s="20"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -3334,9 +3267,8 @@
       <c r="AA28" s="1"/>
       <c r="AB28" s="1"/>
       <c r="AC28" s="25"/>
-      <c r="AD28" s="3"/>
-    </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A29" s="21"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -3366,9 +3298,8 @@
       <c r="AA29" s="3"/>
       <c r="AB29" s="3"/>
       <c r="AC29" s="26"/>
-      <c r="AD29" s="3"/>
-    </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A30" s="20"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -3398,9 +3329,8 @@
       <c r="AA30" s="1"/>
       <c r="AB30" s="1"/>
       <c r="AC30" s="25"/>
-      <c r="AD30" s="3"/>
-    </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A31" s="20"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -3430,9 +3360,8 @@
       <c r="AA31" s="1"/>
       <c r="AB31" s="1"/>
       <c r="AC31" s="25"/>
-      <c r="AD31" s="3"/>
-    </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A32" s="21"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -3462,9 +3391,8 @@
       <c r="AA32" s="3"/>
       <c r="AB32" s="3"/>
       <c r="AC32" s="26"/>
-      <c r="AD32" s="3"/>
-    </row>
-    <row r="33" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A33" s="21"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -3494,9 +3422,8 @@
       <c r="AA33" s="3"/>
       <c r="AB33" s="3"/>
       <c r="AC33" s="26"/>
-      <c r="AD33" s="3"/>
-    </row>
-    <row r="34" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A34" s="20"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -3526,9 +3453,8 @@
       <c r="AA34" s="1"/>
       <c r="AB34" s="1"/>
       <c r="AC34" s="25"/>
-      <c r="AD34" s="3"/>
-    </row>
-    <row r="35" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="35" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A35" s="21"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -3558,9 +3484,8 @@
       <c r="AA35" s="3"/>
       <c r="AB35" s="3"/>
       <c r="AC35" s="26"/>
-      <c r="AD35" s="3"/>
-    </row>
-    <row r="36" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="36" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A36" s="20"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -3590,9 +3515,8 @@
       <c r="AA36" s="1"/>
       <c r="AB36" s="1"/>
       <c r="AC36" s="25"/>
-      <c r="AD36" s="3"/>
-    </row>
-    <row r="37" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="37" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A37" s="21"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -3622,9 +3546,8 @@
       <c r="AA37" s="3"/>
       <c r="AB37" s="3"/>
       <c r="AC37" s="26"/>
-      <c r="AD37" s="3"/>
-    </row>
-    <row r="38" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="38" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A38" s="21"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
@@ -3654,9 +3577,8 @@
       <c r="AA38" s="3"/>
       <c r="AB38" s="3"/>
       <c r="AC38" s="26"/>
-      <c r="AD38" s="3"/>
-    </row>
-    <row r="39" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="39" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A39" s="20"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -3686,9 +3608,8 @@
       <c r="AA39" s="1"/>
       <c r="AB39" s="1"/>
       <c r="AC39" s="25"/>
-      <c r="AD39" s="3"/>
-    </row>
-    <row r="40" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="40" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A40" s="21"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
@@ -3718,9 +3639,8 @@
       <c r="AA40" s="3"/>
       <c r="AB40" s="3"/>
       <c r="AC40" s="26"/>
-      <c r="AD40" s="3"/>
-    </row>
-    <row r="41" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="41" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A41" s="20"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -3750,9 +3670,8 @@
       <c r="AA41" s="1"/>
       <c r="AB41" s="1"/>
       <c r="AC41" s="25"/>
-      <c r="AD41" s="3"/>
-    </row>
-    <row r="42" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="42" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A42" s="21"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
@@ -3782,9 +3701,8 @@
       <c r="AA42" s="3"/>
       <c r="AB42" s="3"/>
       <c r="AC42" s="26"/>
-      <c r="AD42" s="3"/>
-    </row>
-    <row r="43" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="43" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A43" s="20"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -3814,9 +3732,8 @@
       <c r="AA43" s="1"/>
       <c r="AB43" s="1"/>
       <c r="AC43" s="25"/>
-      <c r="AD43" s="3"/>
-    </row>
-    <row r="44" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="44" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A44" s="21"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
@@ -3846,9 +3763,8 @@
       <c r="AA44" s="3"/>
       <c r="AB44" s="3"/>
       <c r="AC44" s="26"/>
-      <c r="AD44" s="3"/>
-    </row>
-    <row r="45" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="45" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A45" s="20"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -3878,9 +3794,8 @@
       <c r="AA45" s="1"/>
       <c r="AB45" s="1"/>
       <c r="AC45" s="25"/>
-      <c r="AD45" s="3"/>
-    </row>
-    <row r="46" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="46" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A46" s="21"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
@@ -3910,9 +3825,8 @@
       <c r="AA46" s="3"/>
       <c r="AB46" s="3"/>
       <c r="AC46" s="26"/>
-      <c r="AD46" s="3"/>
-    </row>
-    <row r="47" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="47" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A47" s="20"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -3942,9 +3856,8 @@
       <c r="AA47" s="1"/>
       <c r="AB47" s="1"/>
       <c r="AC47" s="25"/>
-      <c r="AD47" s="3"/>
-    </row>
-    <row r="48" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="48" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A48" s="21"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
@@ -3974,9 +3887,8 @@
       <c r="AA48" s="3"/>
       <c r="AB48" s="3"/>
       <c r="AC48" s="26"/>
-      <c r="AD48" s="3"/>
-    </row>
-    <row r="49" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="49" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A49" s="20"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -4006,9 +3918,8 @@
       <c r="AA49" s="1"/>
       <c r="AB49" s="1"/>
       <c r="AC49" s="25"/>
-      <c r="AD49" s="3"/>
-    </row>
-    <row r="50" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="50" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A50" s="20"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -4038,9 +3949,8 @@
       <c r="AA50" s="1"/>
       <c r="AB50" s="1"/>
       <c r="AC50" s="25"/>
-      <c r="AD50" s="3"/>
-    </row>
-    <row r="51" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="51" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A51" s="21"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
@@ -4070,9 +3980,8 @@
       <c r="AA51" s="3"/>
       <c r="AB51" s="3"/>
       <c r="AC51" s="26"/>
-      <c r="AD51" s="3"/>
-    </row>
-    <row r="52" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="52" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A52" s="21"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
@@ -4102,9 +4011,8 @@
       <c r="AA52" s="3"/>
       <c r="AB52" s="3"/>
       <c r="AC52" s="26"/>
-      <c r="AD52" s="3"/>
-    </row>
-    <row r="53" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="53" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A53" s="20"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -4134,9 +4042,8 @@
       <c r="AA53" s="1"/>
       <c r="AB53" s="1"/>
       <c r="AC53" s="25"/>
-      <c r="AD53" s="3"/>
-    </row>
-    <row r="54" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="54" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A54" s="20"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -4166,9 +4073,8 @@
       <c r="AA54" s="1"/>
       <c r="AB54" s="1"/>
       <c r="AC54" s="25"/>
-      <c r="AD54" s="3"/>
-    </row>
-    <row r="55" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="55" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A55" s="21"/>
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
@@ -4198,9 +4104,8 @@
       <c r="AA55" s="3"/>
       <c r="AB55" s="3"/>
       <c r="AC55" s="26"/>
-      <c r="AD55" s="3"/>
-    </row>
-    <row r="56" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="56" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A56" s="21"/>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
@@ -4230,9 +4135,8 @@
       <c r="AA56" s="3"/>
       <c r="AB56" s="3"/>
       <c r="AC56" s="26"/>
-      <c r="AD56" s="3"/>
-    </row>
-    <row r="57" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="57" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A57" s="20"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -4262,9 +4166,8 @@
       <c r="AA57" s="1"/>
       <c r="AB57" s="1"/>
       <c r="AC57" s="25"/>
-      <c r="AD57" s="3"/>
-    </row>
-    <row r="58" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="58" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A58" s="20"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -4294,9 +4197,8 @@
       <c r="AA58" s="1"/>
       <c r="AB58" s="1"/>
       <c r="AC58" s="25"/>
-      <c r="AD58" s="3"/>
-    </row>
-    <row r="59" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="59" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A59" s="20"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -4326,9 +4228,8 @@
       <c r="AA59" s="1"/>
       <c r="AB59" s="1"/>
       <c r="AC59" s="25"/>
-      <c r="AD59" s="3"/>
-    </row>
-    <row r="60" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="60" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A60" s="21"/>
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>
@@ -4358,9 +4259,8 @@
       <c r="AA60" s="3"/>
       <c r="AB60" s="3"/>
       <c r="AC60" s="26"/>
-      <c r="AD60" s="3"/>
-    </row>
-    <row r="61" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="61" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A61" s="20"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -4390,9 +4290,8 @@
       <c r="AA61" s="1"/>
       <c r="AB61" s="1"/>
       <c r="AC61" s="25"/>
-      <c r="AD61" s="3"/>
-    </row>
-    <row r="62" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="62" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A62" s="21"/>
       <c r="B62" s="3"/>
       <c r="C62" s="3"/>
@@ -4422,9 +4321,8 @@
       <c r="AA62" s="3"/>
       <c r="AB62" s="3"/>
       <c r="AC62" s="26"/>
-      <c r="AD62" s="3"/>
-    </row>
-    <row r="63" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="63" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A63" s="20"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -4454,9 +4352,8 @@
       <c r="AA63" s="1"/>
       <c r="AB63" s="1"/>
       <c r="AC63" s="25"/>
-      <c r="AD63" s="3"/>
-    </row>
-    <row r="64" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="64" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A64" s="21"/>
       <c r="B64" s="3"/>
       <c r="C64" s="3"/>
@@ -4486,9 +4383,8 @@
       <c r="AA64" s="3"/>
       <c r="AB64" s="3"/>
       <c r="AC64" s="26"/>
-      <c r="AD64" s="3"/>
-    </row>
-    <row r="65" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="65" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A65" s="20"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -4518,9 +4414,8 @@
       <c r="AA65" s="1"/>
       <c r="AB65" s="1"/>
       <c r="AC65" s="25"/>
-      <c r="AD65" s="3"/>
-    </row>
-    <row r="66" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="66" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A66" s="20"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -4550,9 +4445,8 @@
       <c r="AA66" s="1"/>
       <c r="AB66" s="1"/>
       <c r="AC66" s="25"/>
-      <c r="AD66" s="3"/>
-    </row>
-    <row r="67" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="67" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A67" s="20"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -4582,9 +4476,8 @@
       <c r="AA67" s="1"/>
       <c r="AB67" s="1"/>
       <c r="AC67" s="25"/>
-      <c r="AD67" s="3"/>
-    </row>
-    <row r="68" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="68" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A68" s="21"/>
       <c r="B68" s="3"/>
       <c r="C68" s="3"/>
@@ -4614,9 +4507,8 @@
       <c r="AA68" s="3"/>
       <c r="AB68" s="3"/>
       <c r="AC68" s="26"/>
-      <c r="AD68" s="3"/>
-    </row>
-    <row r="69" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="69" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A69" s="20"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -4646,9 +4538,8 @@
       <c r="AA69" s="1"/>
       <c r="AB69" s="1"/>
       <c r="AC69" s="25"/>
-      <c r="AD69" s="3"/>
-    </row>
-    <row r="70" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="70" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A70" s="21"/>
       <c r="B70" s="3"/>
       <c r="C70" s="3"/>
@@ -4678,9 +4569,8 @@
       <c r="AA70" s="3"/>
       <c r="AB70" s="3"/>
       <c r="AC70" s="26"/>
-      <c r="AD70" s="3"/>
-    </row>
-    <row r="71" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="71" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A71" s="20"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -4710,9 +4600,8 @@
       <c r="AA71" s="1"/>
       <c r="AB71" s="1"/>
       <c r="AC71" s="25"/>
-      <c r="AD71" s="3"/>
-    </row>
-    <row r="72" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="72" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A72" s="21"/>
       <c r="B72" s="3"/>
       <c r="C72" s="3"/>
@@ -4742,9 +4631,8 @@
       <c r="AA72" s="3"/>
       <c r="AB72" s="3"/>
       <c r="AC72" s="26"/>
-      <c r="AD72" s="3"/>
-    </row>
-    <row r="73" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="73" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A73" s="21"/>
       <c r="B73" s="3"/>
       <c r="C73" s="3"/>
@@ -4774,9 +4662,8 @@
       <c r="AA73" s="3"/>
       <c r="AB73" s="3"/>
       <c r="AC73" s="26"/>
-      <c r="AD73" s="3"/>
-    </row>
-    <row r="74" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="74" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A74" s="20"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -4806,9 +4693,8 @@
       <c r="AA74" s="1"/>
       <c r="AB74" s="1"/>
       <c r="AC74" s="25"/>
-      <c r="AD74" s="3"/>
-    </row>
-    <row r="75" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="75" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A75" s="21"/>
       <c r="B75" s="3"/>
       <c r="C75" s="3"/>
@@ -4838,9 +4724,8 @@
       <c r="AA75" s="3"/>
       <c r="AB75" s="3"/>
       <c r="AC75" s="26"/>
-      <c r="AD75" s="3"/>
-    </row>
-    <row r="76" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="76" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A76" s="20"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
@@ -4870,9 +4755,8 @@
       <c r="AA76" s="1"/>
       <c r="AB76" s="1"/>
       <c r="AC76" s="25"/>
-      <c r="AD76" s="3"/>
-    </row>
-    <row r="77" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="77" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A77" s="21"/>
       <c r="B77" s="3"/>
       <c r="C77" s="3"/>
@@ -4902,9 +4786,8 @@
       <c r="AA77" s="3"/>
       <c r="AB77" s="3"/>
       <c r="AC77" s="26"/>
-      <c r="AD77" s="3"/>
-    </row>
-    <row r="78" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="78" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A78" s="20"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
@@ -4934,9 +4817,8 @@
       <c r="AA78" s="1"/>
       <c r="AB78" s="1"/>
       <c r="AC78" s="25"/>
-      <c r="AD78" s="3"/>
-    </row>
-    <row r="79" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="79" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A79" s="21"/>
       <c r="B79" s="3"/>
       <c r="C79" s="3"/>
@@ -4966,9 +4848,8 @@
       <c r="AA79" s="3"/>
       <c r="AB79" s="3"/>
       <c r="AC79" s="26"/>
-      <c r="AD79" s="3"/>
-    </row>
-    <row r="80" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="80" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A80" s="20"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
@@ -4998,9 +4879,8 @@
       <c r="AA80" s="1"/>
       <c r="AB80" s="1"/>
       <c r="AC80" s="25"/>
-      <c r="AD80" s="3"/>
-    </row>
-    <row r="81" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="81" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A81" s="20"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
@@ -5030,9 +4910,8 @@
       <c r="AA81" s="1"/>
       <c r="AB81" s="1"/>
       <c r="AC81" s="25"/>
-      <c r="AD81" s="3"/>
-    </row>
-    <row r="82" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="82" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A82" s="20"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
@@ -5062,9 +4941,8 @@
       <c r="AA82" s="1"/>
       <c r="AB82" s="1"/>
       <c r="AC82" s="25"/>
-      <c r="AD82" s="3"/>
-    </row>
-    <row r="83" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="83" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A83" s="21"/>
       <c r="B83" s="3"/>
       <c r="C83" s="3"/>
@@ -5094,9 +4972,8 @@
       <c r="AA83" s="3"/>
       <c r="AB83" s="3"/>
       <c r="AC83" s="26"/>
-      <c r="AD83" s="3"/>
-    </row>
-    <row r="84" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="84" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A84" s="20"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
@@ -5126,9 +5003,8 @@
       <c r="AA84" s="1"/>
       <c r="AB84" s="1"/>
       <c r="AC84" s="25"/>
-      <c r="AD84" s="3"/>
-    </row>
-    <row r="85" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="85" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A85" s="21"/>
       <c r="B85" s="3"/>
       <c r="C85" s="3"/>
@@ -5158,9 +5034,8 @@
       <c r="AA85" s="3"/>
       <c r="AB85" s="3"/>
       <c r="AC85" s="26"/>
-      <c r="AD85" s="3"/>
-    </row>
-    <row r="86" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="86" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A86" s="21"/>
       <c r="B86" s="3"/>
       <c r="C86" s="3"/>
@@ -5190,9 +5065,8 @@
       <c r="AA86" s="3"/>
       <c r="AB86" s="3"/>
       <c r="AC86" s="26"/>
-      <c r="AD86" s="3"/>
-    </row>
-    <row r="87" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="87" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A87" s="21"/>
       <c r="B87" s="3"/>
       <c r="C87" s="3"/>
@@ -5222,9 +5096,8 @@
       <c r="AA87" s="3"/>
       <c r="AB87" s="3"/>
       <c r="AC87" s="26"/>
-      <c r="AD87" s="3"/>
-    </row>
-    <row r="88" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="88" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A88" s="20"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
@@ -5254,9 +5127,8 @@
       <c r="AA88" s="1"/>
       <c r="AB88" s="1"/>
       <c r="AC88" s="25"/>
-      <c r="AD88" s="3"/>
-    </row>
-    <row r="89" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="89" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A89" s="21"/>
       <c r="B89" s="3"/>
       <c r="C89" s="3"/>
@@ -5286,9 +5158,8 @@
       <c r="AA89" s="3"/>
       <c r="AB89" s="3"/>
       <c r="AC89" s="26"/>
-      <c r="AD89" s="3"/>
-    </row>
-    <row r="90" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="90" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A90" s="21"/>
       <c r="B90" s="3"/>
       <c r="C90" s="3"/>
@@ -5318,9 +5189,8 @@
       <c r="AA90" s="3"/>
       <c r="AB90" s="3"/>
       <c r="AC90" s="26"/>
-      <c r="AD90" s="3"/>
-    </row>
-    <row r="91" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="91" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A91" s="41"/>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
@@ -5350,9 +5220,8 @@
       <c r="AA91" s="1"/>
       <c r="AB91" s="1"/>
       <c r="AC91" s="25"/>
-      <c r="AD91" s="3"/>
-    </row>
-    <row r="92" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="92" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A92" s="41"/>
       <c r="B92" s="3"/>
       <c r="C92" s="3"/>
@@ -5382,9 +5251,8 @@
       <c r="AA92" s="3"/>
       <c r="AB92" s="3"/>
       <c r="AC92" s="26"/>
-      <c r="AD92" s="3"/>
-    </row>
-    <row r="93" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="93" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A93" s="41"/>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
@@ -5414,9 +5282,8 @@
       <c r="AA93" s="1"/>
       <c r="AB93" s="1"/>
       <c r="AC93" s="25"/>
-      <c r="AD93" s="3"/>
-    </row>
-    <row r="94" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="94" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A94" s="41"/>
       <c r="B94" s="3"/>
       <c r="C94" s="3"/>
@@ -5446,9 +5313,8 @@
       <c r="AA94" s="3"/>
       <c r="AB94" s="3"/>
       <c r="AC94" s="26"/>
-      <c r="AD94" s="3"/>
-    </row>
-    <row r="95" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="95" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A95" s="41"/>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
@@ -5478,9 +5344,8 @@
       <c r="AA95" s="1"/>
       <c r="AB95" s="1"/>
       <c r="AC95" s="25"/>
-      <c r="AD95" s="3"/>
-    </row>
-    <row r="96" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="96" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A96" s="41"/>
       <c r="B96" s="3"/>
       <c r="C96" s="3"/>
@@ -5510,9 +5375,8 @@
       <c r="AA96" s="3"/>
       <c r="AB96" s="3"/>
       <c r="AC96" s="26"/>
-      <c r="AD96" s="3"/>
-    </row>
-    <row r="97" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="97" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A97" s="41"/>
       <c r="B97" s="3"/>
       <c r="C97" s="3"/>
@@ -5542,9 +5406,8 @@
       <c r="AA97" s="3"/>
       <c r="AB97" s="3"/>
       <c r="AC97" s="26"/>
-      <c r="AD97" s="3"/>
-    </row>
-    <row r="98" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="98" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A98" s="41"/>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
@@ -5574,9 +5437,8 @@
       <c r="AA98" s="1"/>
       <c r="AB98" s="1"/>
       <c r="AC98" s="25"/>
-      <c r="AD98" s="3"/>
-    </row>
-    <row r="99" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="99" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A99" s="41"/>
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
@@ -5606,9 +5468,8 @@
       <c r="AA99" s="1"/>
       <c r="AB99" s="1"/>
       <c r="AC99" s="25"/>
-      <c r="AD99" s="3"/>
-    </row>
-    <row r="100" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="100" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A100" s="40"/>
       <c r="B100" s="3"/>
       <c r="C100" s="3"/>
@@ -5638,9 +5499,8 @@
       <c r="AA100" s="3"/>
       <c r="AB100" s="3"/>
       <c r="AC100" s="26"/>
-      <c r="AD100" s="3"/>
-    </row>
-    <row r="101" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="101" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A101" s="40"/>
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
@@ -5670,9 +5530,8 @@
       <c r="AA101" s="1"/>
       <c r="AB101" s="1"/>
       <c r="AC101" s="25"/>
-      <c r="AD101" s="3"/>
-    </row>
-    <row r="102" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="102" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A102" s="40"/>
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
@@ -5702,9 +5561,8 @@
       <c r="AA102" s="1"/>
       <c r="AB102" s="1"/>
       <c r="AC102" s="25"/>
-      <c r="AD102" s="3"/>
-    </row>
-    <row r="103" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="103" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A103" s="21"/>
       <c r="B103" s="3"/>
       <c r="C103" s="3"/>
@@ -5734,9 +5592,8 @@
       <c r="AA103" s="3"/>
       <c r="AB103" s="3"/>
       <c r="AC103" s="26"/>
-      <c r="AD103" s="3"/>
-    </row>
-    <row r="104" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="104" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A104" s="20"/>
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
@@ -5766,9 +5623,8 @@
       <c r="AA104" s="1"/>
       <c r="AB104" s="1"/>
       <c r="AC104" s="25"/>
-      <c r="AD104" s="3"/>
-    </row>
-    <row r="105" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="105" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A105" s="21"/>
       <c r="B105" s="3"/>
       <c r="C105" s="3"/>
@@ -5798,9 +5654,8 @@
       <c r="AA105" s="3"/>
       <c r="AB105" s="3"/>
       <c r="AC105" s="26"/>
-      <c r="AD105" s="3"/>
-    </row>
-    <row r="106" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="106" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A106" s="20"/>
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
@@ -5830,9 +5685,8 @@
       <c r="AA106" s="1"/>
       <c r="AB106" s="1"/>
       <c r="AC106" s="25"/>
-      <c r="AD106" s="3"/>
-    </row>
-    <row r="107" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="107" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A107" s="21"/>
       <c r="B107" s="3"/>
       <c r="C107" s="3"/>
@@ -5862,9 +5716,8 @@
       <c r="AA107" s="3"/>
       <c r="AB107" s="3"/>
       <c r="AC107" s="26"/>
-      <c r="AD107" s="3"/>
-    </row>
-    <row r="108" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="108" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A108" s="20"/>
       <c r="B108" s="1"/>
       <c r="C108" s="1"/>
@@ -5894,9 +5747,8 @@
       <c r="AA108" s="1"/>
       <c r="AB108" s="1"/>
       <c r="AC108" s="25"/>
-      <c r="AD108" s="3"/>
-    </row>
-    <row r="109" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="109" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A109" s="21"/>
       <c r="B109" s="3"/>
       <c r="C109" s="3"/>
@@ -5926,9 +5778,8 @@
       <c r="AA109" s="3"/>
       <c r="AB109" s="3"/>
       <c r="AC109" s="26"/>
-      <c r="AD109" s="3"/>
-    </row>
-    <row r="110" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="110" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A110" s="20"/>
       <c r="B110" s="1"/>
       <c r="C110" s="1"/>
@@ -5958,9 +5809,8 @@
       <c r="AA110" s="1"/>
       <c r="AB110" s="1"/>
       <c r="AC110" s="25"/>
-      <c r="AD110" s="3"/>
-    </row>
-    <row r="111" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="111" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A111" s="21"/>
       <c r="B111" s="3"/>
       <c r="C111" s="3"/>
@@ -5990,9 +5840,8 @@
       <c r="AA111" s="3"/>
       <c r="AB111" s="3"/>
       <c r="AC111" s="26"/>
-      <c r="AD111" s="3"/>
-    </row>
-    <row r="112" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="112" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A112" s="20"/>
       <c r="B112" s="1"/>
       <c r="C112" s="1"/>
@@ -6022,9 +5871,8 @@
       <c r="AA112" s="1"/>
       <c r="AB112" s="1"/>
       <c r="AC112" s="25"/>
-      <c r="AD112" s="3"/>
-    </row>
-    <row r="113" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="113" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A113" s="21"/>
       <c r="B113" s="3"/>
       <c r="C113" s="3"/>
@@ -6054,9 +5902,8 @@
       <c r="AA113" s="3"/>
       <c r="AB113" s="3"/>
       <c r="AC113" s="26"/>
-      <c r="AD113" s="3"/>
-    </row>
-    <row r="114" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="114" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A114" s="20"/>
       <c r="B114" s="1"/>
       <c r="C114" s="1"/>
@@ -6086,9 +5933,8 @@
       <c r="AA114" s="1"/>
       <c r="AB114" s="1"/>
       <c r="AC114" s="25"/>
-      <c r="AD114" s="3"/>
-    </row>
-    <row r="115" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="115" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A115" s="21"/>
       <c r="B115" s="3"/>
       <c r="C115" s="3"/>
@@ -6118,9 +5964,8 @@
       <c r="AA115" s="3"/>
       <c r="AB115" s="3"/>
       <c r="AC115" s="26"/>
-      <c r="AD115" s="3"/>
-    </row>
-    <row r="116" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="116" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A116" s="20"/>
       <c r="B116" s="1"/>
       <c r="C116" s="1"/>
@@ -6150,9 +5995,8 @@
       <c r="AA116" s="1"/>
       <c r="AB116" s="1"/>
       <c r="AC116" s="25"/>
-      <c r="AD116" s="3"/>
-    </row>
-    <row r="117" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="117" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A117" s="21"/>
       <c r="B117" s="3"/>
       <c r="C117" s="3"/>
@@ -6182,9 +6026,8 @@
       <c r="AA117" s="3"/>
       <c r="AB117" s="3"/>
       <c r="AC117" s="26"/>
-      <c r="AD117" s="3"/>
-    </row>
-    <row r="118" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="118" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A118" s="20"/>
       <c r="B118" s="1"/>
       <c r="C118" s="1"/>
@@ -6214,9 +6057,8 @@
       <c r="AA118" s="1"/>
       <c r="AB118" s="1"/>
       <c r="AC118" s="25"/>
-      <c r="AD118" s="3"/>
-    </row>
-    <row r="119" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="119" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A119" s="21"/>
       <c r="B119" s="3"/>
       <c r="C119" s="3"/>
@@ -6246,9 +6088,8 @@
       <c r="AA119" s="3"/>
       <c r="AB119" s="3"/>
       <c r="AC119" s="26"/>
-      <c r="AD119" s="3"/>
-    </row>
-    <row r="120" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="120" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A120" s="20"/>
       <c r="B120" s="1"/>
       <c r="C120" s="1"/>
@@ -6278,9 +6119,8 @@
       <c r="AA120" s="1"/>
       <c r="AB120" s="1"/>
       <c r="AC120" s="25"/>
-      <c r="AD120" s="3"/>
-    </row>
-    <row r="121" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="121" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A121" s="21"/>
       <c r="B121" s="3"/>
       <c r="C121" s="3"/>
@@ -6310,9 +6150,8 @@
       <c r="AA121" s="3"/>
       <c r="AB121" s="3"/>
       <c r="AC121" s="26"/>
-      <c r="AD121" s="3"/>
-    </row>
-    <row r="122" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="122" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A122" s="20"/>
       <c r="B122" s="1"/>
       <c r="C122" s="1"/>
@@ -6342,9 +6181,8 @@
       <c r="AA122" s="1"/>
       <c r="AB122" s="1"/>
       <c r="AC122" s="25"/>
-      <c r="AD122" s="3"/>
-    </row>
-    <row r="123" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="123" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A123" s="21"/>
       <c r="B123" s="3"/>
       <c r="C123" s="3"/>
@@ -6374,9 +6212,8 @@
       <c r="AA123" s="3"/>
       <c r="AB123" s="3"/>
       <c r="AC123" s="26"/>
-      <c r="AD123" s="3"/>
-    </row>
-    <row r="124" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="124" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A124" s="20"/>
       <c r="B124" s="1"/>
       <c r="C124" s="1"/>
@@ -6406,9 +6243,8 @@
       <c r="AA124" s="1"/>
       <c r="AB124" s="1"/>
       <c r="AC124" s="25"/>
-      <c r="AD124" s="3"/>
-    </row>
-    <row r="125" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="125" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A125" s="21"/>
       <c r="B125" s="3"/>
       <c r="C125" s="3"/>
@@ -6438,9 +6274,8 @@
       <c r="AA125" s="3"/>
       <c r="AB125" s="3"/>
       <c r="AC125" s="26"/>
-      <c r="AD125" s="3"/>
-    </row>
-    <row r="126" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="126" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A126" s="20"/>
       <c r="B126" s="1"/>
       <c r="C126" s="1"/>
@@ -6470,9 +6305,8 @@
       <c r="AA126" s="1"/>
       <c r="AB126" s="1"/>
       <c r="AC126" s="25"/>
-      <c r="AD126" s="3"/>
-    </row>
-    <row r="127" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="127" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A127" s="21"/>
       <c r="B127" s="3"/>
       <c r="C127" s="3"/>
@@ -6502,9 +6336,8 @@
       <c r="AA127" s="3"/>
       <c r="AB127" s="3"/>
       <c r="AC127" s="26"/>
-      <c r="AD127" s="3"/>
-    </row>
-    <row r="128" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="128" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A128" s="20"/>
       <c r="B128" s="1"/>
       <c r="C128" s="1"/>
@@ -6534,9 +6367,8 @@
       <c r="AA128" s="1"/>
       <c r="AB128" s="1"/>
       <c r="AC128" s="25"/>
-      <c r="AD128" s="3"/>
-    </row>
-    <row r="129" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="129" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A129" s="21"/>
       <c r="B129" s="3"/>
       <c r="C129" s="3"/>
@@ -6566,9 +6398,8 @@
       <c r="AA129" s="3"/>
       <c r="AB129" s="3"/>
       <c r="AC129" s="26"/>
-      <c r="AD129" s="3"/>
-    </row>
-    <row r="130" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="130" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A130" s="20"/>
       <c r="B130" s="1"/>
       <c r="C130" s="1"/>
@@ -6598,9 +6429,8 @@
       <c r="AA130" s="1"/>
       <c r="AB130" s="1"/>
       <c r="AC130" s="25"/>
-      <c r="AD130" s="3"/>
-    </row>
-    <row r="131" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="131" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A131" s="21"/>
       <c r="B131" s="3"/>
       <c r="C131" s="3"/>
@@ -6630,9 +6460,8 @@
       <c r="AA131" s="3"/>
       <c r="AB131" s="3"/>
       <c r="AC131" s="26"/>
-      <c r="AD131" s="3"/>
-    </row>
-    <row r="132" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="132" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A132" s="20"/>
       <c r="B132" s="1"/>
       <c r="C132" s="1"/>
@@ -6662,9 +6491,8 @@
       <c r="AA132" s="1"/>
       <c r="AB132" s="1"/>
       <c r="AC132" s="25"/>
-      <c r="AD132" s="3"/>
-    </row>
-    <row r="133" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="133" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A133" s="21"/>
       <c r="B133" s="3"/>
       <c r="C133" s="3"/>
@@ -6694,9 +6522,8 @@
       <c r="AA133" s="3"/>
       <c r="AB133" s="3"/>
       <c r="AC133" s="26"/>
-      <c r="AD133" s="3"/>
-    </row>
-    <row r="134" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="134" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A134" s="20"/>
       <c r="B134" s="1"/>
       <c r="C134" s="1"/>
@@ -6726,9 +6553,8 @@
       <c r="AA134" s="1"/>
       <c r="AB134" s="1"/>
       <c r="AC134" s="25"/>
-      <c r="AD134" s="3"/>
-    </row>
-    <row r="135" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="135" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A135" s="21"/>
       <c r="B135" s="3"/>
       <c r="C135" s="3"/>
@@ -6758,9 +6584,8 @@
       <c r="AA135" s="3"/>
       <c r="AB135" s="3"/>
       <c r="AC135" s="26"/>
-      <c r="AD135" s="3"/>
-    </row>
-    <row r="136" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="136" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A136" s="20"/>
       <c r="B136" s="1"/>
       <c r="C136" s="1"/>
@@ -6790,9 +6615,8 @@
       <c r="AA136" s="1"/>
       <c r="AB136" s="1"/>
       <c r="AC136" s="25"/>
-      <c r="AD136" s="3"/>
-    </row>
-    <row r="137" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="137" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A137" s="21"/>
       <c r="B137" s="3"/>
       <c r="C137" s="3"/>
@@ -6822,9 +6646,8 @@
       <c r="AA137" s="3"/>
       <c r="AB137" s="3"/>
       <c r="AC137" s="26"/>
-      <c r="AD137" s="3"/>
-    </row>
-    <row r="138" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="138" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A138" s="20"/>
       <c r="B138" s="1"/>
       <c r="C138" s="1"/>
@@ -6854,9 +6677,8 @@
       <c r="AA138" s="1"/>
       <c r="AB138" s="1"/>
       <c r="AC138" s="25"/>
-      <c r="AD138" s="3"/>
-    </row>
-    <row r="139" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="139" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A139" s="21"/>
       <c r="B139" s="3"/>
       <c r="C139" s="3"/>
@@ -6886,9 +6708,8 @@
       <c r="AA139" s="3"/>
       <c r="AB139" s="3"/>
       <c r="AC139" s="26"/>
-      <c r="AD139" s="3"/>
-    </row>
-    <row r="140" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="140" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A140" s="20"/>
       <c r="B140" s="1"/>
       <c r="C140" s="1"/>
@@ -6918,9 +6739,8 @@
       <c r="AA140" s="1"/>
       <c r="AB140" s="1"/>
       <c r="AC140" s="25"/>
-      <c r="AD140" s="3"/>
-    </row>
-    <row r="141" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="141" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A141" s="21"/>
       <c r="B141" s="3"/>
       <c r="C141" s="3"/>
@@ -6950,9 +6770,8 @@
       <c r="AA141" s="3"/>
       <c r="AB141" s="3"/>
       <c r="AC141" s="26"/>
-      <c r="AD141" s="3"/>
-    </row>
-    <row r="142" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="142" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A142" s="20"/>
       <c r="B142" s="1"/>
       <c r="C142" s="1"/>
@@ -6982,9 +6801,8 @@
       <c r="AA142" s="1"/>
       <c r="AB142" s="1"/>
       <c r="AC142" s="25"/>
-      <c r="AD142" s="3"/>
-    </row>
-    <row r="143" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="143" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A143" s="21"/>
       <c r="B143" s="3"/>
       <c r="C143" s="3"/>
@@ -7014,9 +6832,8 @@
       <c r="AA143" s="3"/>
       <c r="AB143" s="3"/>
       <c r="AC143" s="26"/>
-      <c r="AD143" s="3"/>
-    </row>
-    <row r="144" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="144" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A144" s="20"/>
       <c r="B144" s="1"/>
       <c r="C144" s="1"/>
@@ -7046,9 +6863,8 @@
       <c r="AA144" s="1"/>
       <c r="AB144" s="1"/>
       <c r="AC144" s="25"/>
-      <c r="AD144" s="3"/>
-    </row>
-    <row r="145" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="145" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A145" s="21"/>
       <c r="B145" s="3"/>
       <c r="C145" s="3"/>
@@ -7078,9 +6894,8 @@
       <c r="AA145" s="3"/>
       <c r="AB145" s="3"/>
       <c r="AC145" s="26"/>
-      <c r="AD145" s="3"/>
-    </row>
-    <row r="146" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="146" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A146" s="20"/>
       <c r="B146" s="1"/>
       <c r="C146" s="1"/>
@@ -7110,9 +6925,8 @@
       <c r="AA146" s="1"/>
       <c r="AB146" s="1"/>
       <c r="AC146" s="25"/>
-      <c r="AD146" s="3"/>
-    </row>
-    <row r="147" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="147" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A147" s="21"/>
       <c r="B147" s="3"/>
       <c r="C147" s="3"/>
@@ -7142,9 +6956,8 @@
       <c r="AA147" s="3"/>
       <c r="AB147" s="3"/>
       <c r="AC147" s="26"/>
-      <c r="AD147" s="3"/>
-    </row>
-    <row r="148" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="148" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A148" s="20"/>
       <c r="B148" s="1"/>
       <c r="C148" s="1"/>
@@ -7174,9 +6987,8 @@
       <c r="AA148" s="1"/>
       <c r="AB148" s="1"/>
       <c r="AC148" s="25"/>
-      <c r="AD148" s="3"/>
-    </row>
-    <row r="149" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="149" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A149" s="21"/>
       <c r="B149" s="3"/>
       <c r="C149" s="3"/>
@@ -7206,9 +7018,8 @@
       <c r="AA149" s="3"/>
       <c r="AB149" s="3"/>
       <c r="AC149" s="26"/>
-      <c r="AD149" s="3"/>
-    </row>
-    <row r="150" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="150" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A150" s="21"/>
       <c r="B150" s="3"/>
       <c r="C150" s="3"/>
@@ -7238,9 +7049,8 @@
       <c r="AA150" s="3"/>
       <c r="AB150" s="3"/>
       <c r="AC150" s="26"/>
-      <c r="AD150" s="3"/>
-    </row>
-    <row r="151" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="151" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A151" s="21"/>
       <c r="B151" s="3"/>
       <c r="C151" s="3"/>
@@ -7270,9 +7080,8 @@
       <c r="AA151" s="3"/>
       <c r="AB151" s="3"/>
       <c r="AC151" s="26"/>
-      <c r="AD151" s="3"/>
-    </row>
-    <row r="152" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="152" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A152" s="21"/>
       <c r="B152" s="3"/>
       <c r="C152" s="3"/>
@@ -7302,9 +7111,8 @@
       <c r="AA152" s="3"/>
       <c r="AB152" s="3"/>
       <c r="AC152" s="26"/>
-      <c r="AD152" s="3"/>
-    </row>
-    <row r="153" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="153" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A153" s="20"/>
       <c r="B153" s="1"/>
       <c r="C153" s="1"/>
@@ -7334,9 +7142,8 @@
       <c r="AA153" s="1"/>
       <c r="AB153" s="1"/>
       <c r="AC153" s="25"/>
-      <c r="AD153" s="3"/>
-    </row>
-    <row r="154" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="154" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A154" s="22"/>
       <c r="B154" s="3"/>
       <c r="C154" s="11"/>
@@ -7366,9 +7173,8 @@
       <c r="AA154" s="3"/>
       <c r="AB154" s="3"/>
       <c r="AC154" s="26"/>
-      <c r="AD154" s="3"/>
-    </row>
-    <row r="155" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="155" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A155" s="22"/>
       <c r="B155" s="1"/>
       <c r="C155" s="11"/>
@@ -7398,9 +7204,8 @@
       <c r="AA155" s="1"/>
       <c r="AB155" s="1"/>
       <c r="AC155" s="25"/>
-      <c r="AD155" s="3"/>
-    </row>
-    <row r="156" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="156" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A156" s="22"/>
       <c r="B156" s="3"/>
       <c r="C156" s="11"/>
@@ -7430,9 +7235,8 @@
       <c r="AA156" s="3"/>
       <c r="AB156" s="3"/>
       <c r="AC156" s="26"/>
-      <c r="AD156" s="3"/>
-    </row>
-    <row r="157" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="157" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A157" s="22"/>
       <c r="B157" s="1"/>
       <c r="C157" s="11"/>
@@ -7462,9 +7266,8 @@
       <c r="AA157" s="1"/>
       <c r="AB157" s="1"/>
       <c r="AC157" s="25"/>
-      <c r="AD157" s="3"/>
-    </row>
-    <row r="158" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="158" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A158" s="22"/>
       <c r="B158" s="3"/>
       <c r="C158" s="11"/>
@@ -7494,9 +7297,8 @@
       <c r="AA158" s="3"/>
       <c r="AB158" s="3"/>
       <c r="AC158" s="26"/>
-      <c r="AD158" s="3"/>
-    </row>
-    <row r="159" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="159" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A159" s="22"/>
       <c r="B159" s="1"/>
       <c r="C159" s="11"/>
@@ -7526,9 +7328,8 @@
       <c r="AA159" s="1"/>
       <c r="AB159" s="1"/>
       <c r="AC159" s="25"/>
-      <c r="AD159" s="3"/>
-    </row>
-    <row r="160" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="160" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A160" s="22"/>
       <c r="B160" s="3"/>
       <c r="C160" s="11"/>
@@ -7558,9 +7359,8 @@
       <c r="AA160" s="3"/>
       <c r="AB160" s="3"/>
       <c r="AC160" s="26"/>
-      <c r="AD160" s="3"/>
-    </row>
-    <row r="161" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="161" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A161" s="23"/>
       <c r="B161" s="1"/>
       <c r="C161" s="11"/>
@@ -7590,9 +7390,8 @@
       <c r="AA161" s="1"/>
       <c r="AB161" s="14"/>
       <c r="AC161" s="25"/>
-      <c r="AD161" s="3"/>
-    </row>
-    <row r="162" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="162" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A162" s="23"/>
       <c r="B162" s="3"/>
       <c r="C162" s="11"/>
@@ -7622,9 +7421,8 @@
       <c r="AA162" s="3"/>
       <c r="AB162" s="15"/>
       <c r="AC162" s="26"/>
-      <c r="AD162" s="3"/>
-    </row>
-    <row r="163" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="163" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A163" s="23"/>
       <c r="B163" s="1"/>
       <c r="C163" s="11"/>
@@ -7654,9 +7452,8 @@
       <c r="AA163" s="1"/>
       <c r="AB163" s="14"/>
       <c r="AC163" s="25"/>
-      <c r="AD163" s="3"/>
-    </row>
-    <row r="164" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="164" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A164" s="23"/>
       <c r="B164" s="3"/>
       <c r="C164" s="11"/>
@@ -7686,9 +7483,8 @@
       <c r="AA164" s="3"/>
       <c r="AB164" s="15"/>
       <c r="AC164" s="26"/>
-      <c r="AD164" s="3"/>
-    </row>
-    <row r="165" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="165" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A165" s="23"/>
       <c r="B165" s="1"/>
       <c r="C165" s="11"/>
@@ -7718,9 +7514,8 @@
       <c r="AA165" s="1"/>
       <c r="AB165" s="14"/>
       <c r="AC165" s="25"/>
-      <c r="AD165" s="3"/>
-    </row>
-    <row r="166" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="166" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A166" s="23"/>
       <c r="B166" s="3"/>
       <c r="C166" s="11"/>
@@ -7750,9 +7545,8 @@
       <c r="AA166" s="3"/>
       <c r="AB166" s="15"/>
       <c r="AC166" s="26"/>
-      <c r="AD166" s="3"/>
-    </row>
-    <row r="167" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="167" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A167" s="23"/>
       <c r="B167" s="1"/>
       <c r="C167" s="11"/>
@@ -7782,9 +7576,8 @@
       <c r="AA167" s="1"/>
       <c r="AB167" s="14"/>
       <c r="AC167" s="25"/>
-      <c r="AD167" s="3"/>
-    </row>
-    <row r="168" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="168" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A168" s="23"/>
       <c r="B168" s="3"/>
       <c r="C168" s="11"/>
@@ -7814,9 +7607,8 @@
       <c r="AA168" s="3"/>
       <c r="AB168" s="15"/>
       <c r="AC168" s="26"/>
-      <c r="AD168" s="3"/>
-    </row>
-    <row r="169" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="169" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A169" s="23"/>
       <c r="B169" s="1"/>
       <c r="C169" s="11"/>
@@ -7846,9 +7638,8 @@
       <c r="AA169" s="1"/>
       <c r="AB169" s="14"/>
       <c r="AC169" s="25"/>
-      <c r="AD169" s="3"/>
-    </row>
-    <row r="170" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="170" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A170" s="22"/>
       <c r="B170" s="3"/>
       <c r="C170" s="11"/>
@@ -7878,9 +7669,8 @@
       <c r="AA170" s="3"/>
       <c r="AB170" s="15"/>
       <c r="AC170" s="26"/>
-      <c r="AD170" s="3"/>
-    </row>
-    <row r="171" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="171" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A171" s="22"/>
       <c r="B171" s="1"/>
       <c r="C171" s="11"/>
@@ -7910,9 +7700,8 @@
       <c r="AA171" s="1"/>
       <c r="AB171" s="14"/>
       <c r="AC171" s="25"/>
-      <c r="AD171" s="3"/>
-    </row>
-    <row r="172" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="172" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A172" s="22"/>
       <c r="B172" s="3"/>
       <c r="C172" s="11"/>
@@ -7942,9 +7731,8 @@
       <c r="AA172" s="3"/>
       <c r="AB172" s="15"/>
       <c r="AC172" s="26"/>
-      <c r="AD172" s="3"/>
-    </row>
-    <row r="173" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="173" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A173" s="22"/>
       <c r="B173" s="1"/>
       <c r="C173" s="11"/>
@@ -7974,9 +7762,8 @@
       <c r="AA173" s="1"/>
       <c r="AB173" s="14"/>
       <c r="AC173" s="25"/>
-      <c r="AD173" s="3"/>
-    </row>
-    <row r="174" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="174" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A174" s="22"/>
       <c r="B174" s="3"/>
       <c r="C174" s="11"/>
@@ -8006,9 +7793,8 @@
       <c r="AA174" s="3"/>
       <c r="AB174" s="15"/>
       <c r="AC174" s="26"/>
-      <c r="AD174" s="3"/>
-    </row>
-    <row r="175" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="175" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A175" s="22"/>
       <c r="B175" s="1"/>
       <c r="C175" s="11"/>
@@ -8038,9 +7824,8 @@
       <c r="AA175" s="1"/>
       <c r="AB175" s="14"/>
       <c r="AC175" s="25"/>
-      <c r="AD175" s="3"/>
-    </row>
-    <row r="176" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="176" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A176" s="22"/>
       <c r="B176" s="3"/>
       <c r="C176" s="11"/>
@@ -8070,9 +7855,8 @@
       <c r="AA176" s="3"/>
       <c r="AB176" s="15"/>
       <c r="AC176" s="26"/>
-      <c r="AD176" s="3"/>
-    </row>
-    <row r="177" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="177" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A177" s="22"/>
       <c r="B177" s="1"/>
       <c r="C177" s="11"/>
@@ -8102,9 +7886,8 @@
       <c r="AA177" s="1"/>
       <c r="AB177" s="14"/>
       <c r="AC177" s="25"/>
-      <c r="AD177" s="3"/>
-    </row>
-    <row r="178" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="178" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A178" s="22"/>
       <c r="B178" s="3"/>
       <c r="C178" s="11"/>
@@ -8134,9 +7917,8 @@
       <c r="AA178" s="3"/>
       <c r="AB178" s="15"/>
       <c r="AC178" s="26"/>
-      <c r="AD178" s="3"/>
-    </row>
-    <row r="179" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="179" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A179" s="22"/>
       <c r="B179" s="1"/>
       <c r="C179" s="11"/>
@@ -8166,9 +7948,8 @@
       <c r="AA179" s="1"/>
       <c r="AB179" s="14"/>
       <c r="AC179" s="25"/>
-      <c r="AD179" s="3"/>
-    </row>
-    <row r="180" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="180" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A180" s="22"/>
       <c r="B180" s="3"/>
       <c r="C180" s="11"/>
@@ -8198,9 +7979,8 @@
       <c r="AA180" s="3"/>
       <c r="AB180" s="15"/>
       <c r="AC180" s="26"/>
-      <c r="AD180" s="3"/>
-    </row>
-    <row r="181" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="181" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A181" s="22"/>
       <c r="B181" s="1"/>
       <c r="C181" s="11"/>
@@ -8230,9 +8010,8 @@
       <c r="AA181" s="1"/>
       <c r="AB181" s="14"/>
       <c r="AC181" s="25"/>
-      <c r="AD181" s="3"/>
-    </row>
-    <row r="182" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="182" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A182" s="22"/>
       <c r="B182" s="3"/>
       <c r="C182" s="11"/>
@@ -8262,9 +8041,8 @@
       <c r="AA182" s="3"/>
       <c r="AB182" s="15"/>
       <c r="AC182" s="26"/>
-      <c r="AD182" s="3"/>
-    </row>
-    <row r="183" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="183" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A183" s="22"/>
       <c r="B183" s="1"/>
       <c r="C183" s="11"/>
@@ -8294,9 +8072,8 @@
       <c r="AA183" s="1"/>
       <c r="AB183" s="14"/>
       <c r="AC183" s="25"/>
-      <c r="AD183" s="3"/>
-    </row>
-    <row r="184" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="184" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A184" s="22"/>
       <c r="B184" s="3"/>
       <c r="C184" s="11"/>
@@ -8326,9 +8103,8 @@
       <c r="AA184" s="3"/>
       <c r="AB184" s="3"/>
       <c r="AC184" s="26"/>
-      <c r="AD184" s="3"/>
-    </row>
-    <row r="185" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="185" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A185" s="22"/>
       <c r="B185" s="1"/>
       <c r="C185" s="11"/>
@@ -8358,9 +8134,8 @@
       <c r="AA185" s="1"/>
       <c r="AB185" s="1"/>
       <c r="AC185" s="25"/>
-      <c r="AD185" s="3"/>
-    </row>
-    <row r="186" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="186" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A186" s="22"/>
       <c r="B186" s="3"/>
       <c r="C186" s="11"/>
@@ -8390,9 +8165,8 @@
       <c r="AA186" s="3"/>
       <c r="AB186" s="3"/>
       <c r="AC186" s="26"/>
-      <c r="AD186" s="3"/>
-    </row>
-    <row r="187" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="187" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A187" s="22"/>
       <c r="B187" s="1"/>
       <c r="C187" s="11"/>
@@ -8422,9 +8196,8 @@
       <c r="AA187" s="1"/>
       <c r="AB187" s="14"/>
       <c r="AC187" s="25"/>
-      <c r="AD187" s="3"/>
-    </row>
-    <row r="188" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="188" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A188" s="22"/>
       <c r="B188" s="3"/>
       <c r="C188" s="11"/>
@@ -8454,9 +8227,8 @@
       <c r="AA188" s="3"/>
       <c r="AB188" s="3"/>
       <c r="AC188" s="26"/>
-      <c r="AD188" s="3"/>
-    </row>
-    <row r="189" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="189" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A189" s="22"/>
       <c r="B189" s="1"/>
       <c r="C189" s="11"/>
@@ -8486,9 +8258,8 @@
       <c r="AA189" s="1"/>
       <c r="AB189" s="14"/>
       <c r="AC189" s="25"/>
-      <c r="AD189" s="3"/>
-    </row>
-    <row r="190" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="190" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A190" s="24"/>
       <c r="B190" s="3"/>
       <c r="C190" s="3"/>
@@ -8518,9 +8289,8 @@
       <c r="AA190" s="3"/>
       <c r="AB190" s="3"/>
       <c r="AC190" s="26"/>
-      <c r="AD190" s="3"/>
-    </row>
-    <row r="191" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="191" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A191" s="24"/>
       <c r="B191" s="1"/>
       <c r="C191" s="1"/>
@@ -8550,9 +8320,8 @@
       <c r="AA191" s="1"/>
       <c r="AB191" s="1"/>
       <c r="AC191" s="25"/>
-      <c r="AD191" s="3"/>
-    </row>
-    <row r="192" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="192" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A192" s="24"/>
       <c r="B192" s="3"/>
       <c r="C192" s="3"/>
@@ -8582,9 +8351,8 @@
       <c r="AA192" s="3"/>
       <c r="AB192" s="3"/>
       <c r="AC192" s="26"/>
-      <c r="AD192" s="3"/>
-    </row>
-    <row r="193" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="193" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A193" s="24"/>
       <c r="B193" s="1"/>
       <c r="C193" s="1"/>
@@ -8614,9 +8382,8 @@
       <c r="AA193" s="1"/>
       <c r="AB193" s="1"/>
       <c r="AC193" s="25"/>
-      <c r="AD193" s="3"/>
-    </row>
-    <row r="194" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="194" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A194" s="24"/>
       <c r="B194" s="3"/>
       <c r="C194" s="3"/>
@@ -8646,9 +8413,8 @@
       <c r="AA194" s="3"/>
       <c r="AB194" s="3"/>
       <c r="AC194" s="26"/>
-      <c r="AD194" s="3"/>
-    </row>
-    <row r="195" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="195" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A195" s="24"/>
       <c r="B195" s="1"/>
       <c r="C195" s="1"/>
@@ -8678,9 +8444,8 @@
       <c r="AA195" s="1"/>
       <c r="AB195" s="1"/>
       <c r="AC195" s="25"/>
-      <c r="AD195" s="3"/>
-    </row>
-    <row r="196" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="196" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A196" s="24"/>
       <c r="B196" s="3"/>
       <c r="C196" s="3"/>
@@ -8710,9 +8475,8 @@
       <c r="AA196" s="3"/>
       <c r="AB196" s="3"/>
       <c r="AC196" s="26"/>
-      <c r="AD196" s="3"/>
-    </row>
-    <row r="197" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="197" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A197" s="24"/>
       <c r="B197" s="1"/>
       <c r="C197" s="1"/>
@@ -8742,9 +8506,8 @@
       <c r="AA197" s="1"/>
       <c r="AB197" s="1"/>
       <c r="AC197" s="25"/>
-      <c r="AD197" s="3"/>
-    </row>
-    <row r="198" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="198" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A198" s="24"/>
       <c r="B198" s="3"/>
       <c r="C198" s="3"/>
@@ -8774,9 +8537,8 @@
       <c r="AA198" s="3"/>
       <c r="AB198" s="3"/>
       <c r="AC198" s="26"/>
-      <c r="AD198" s="3"/>
-    </row>
-    <row r="199" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="199" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A199" s="24"/>
       <c r="B199" s="1"/>
       <c r="C199" s="1"/>
@@ -8806,9 +8568,8 @@
       <c r="AA199" s="1"/>
       <c r="AB199" s="1"/>
       <c r="AC199" s="25"/>
-      <c r="AD199" s="3"/>
-    </row>
-    <row r="200" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="200" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A200" s="24"/>
       <c r="B200" s="3"/>
       <c r="C200" s="3"/>
@@ -8838,9 +8599,8 @@
       <c r="AA200" s="3"/>
       <c r="AB200" s="3"/>
       <c r="AC200" s="26"/>
-      <c r="AD200" s="3"/>
-    </row>
-    <row r="201" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="201" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A201" s="24"/>
       <c r="B201" s="1"/>
       <c r="C201" s="1"/>
@@ -8870,9 +8630,8 @@
       <c r="AA201" s="1"/>
       <c r="AB201" s="1"/>
       <c r="AC201" s="25"/>
-      <c r="AD201" s="3"/>
-    </row>
-    <row r="202" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="202" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A202" s="24"/>
       <c r="B202" s="3"/>
       <c r="C202" s="3"/>
@@ -8902,9 +8661,8 @@
       <c r="AA202" s="3"/>
       <c r="AB202" s="3"/>
       <c r="AC202" s="26"/>
-      <c r="AD202" s="3"/>
-    </row>
-    <row r="203" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="203" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A203" s="24"/>
       <c r="B203" s="1"/>
       <c r="C203" s="1"/>
@@ -8934,9 +8692,8 @@
       <c r="AA203" s="1"/>
       <c r="AB203" s="1"/>
       <c r="AC203" s="25"/>
-      <c r="AD203" s="3"/>
-    </row>
-    <row r="204" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="204" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A204" s="24"/>
       <c r="B204" s="3"/>
       <c r="C204" s="3"/>
@@ -8966,9 +8723,8 @@
       <c r="AA204" s="3"/>
       <c r="AB204" s="3"/>
       <c r="AC204" s="26"/>
-      <c r="AD204" s="3"/>
-    </row>
-    <row r="205" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="205" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A205" s="20"/>
       <c r="B205" s="1"/>
       <c r="C205" s="1"/>
@@ -8998,9 +8754,8 @@
       <c r="AA205" s="1"/>
       <c r="AB205" s="1"/>
       <c r="AC205" s="25"/>
-      <c r="AD205" s="3"/>
-    </row>
-    <row r="206" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="206" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A206" s="21"/>
       <c r="B206" s="1"/>
       <c r="C206" s="1"/>
@@ -9030,9 +8785,8 @@
       <c r="AA206" s="3"/>
       <c r="AB206" s="3"/>
       <c r="AC206" s="26"/>
-      <c r="AD206" s="3"/>
-    </row>
-    <row r="207" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="207" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A207" s="20"/>
       <c r="B207" s="1"/>
       <c r="C207" s="1"/>
@@ -9062,9 +8816,8 @@
       <c r="AA207" s="1"/>
       <c r="AB207" s="1"/>
       <c r="AC207" s="25"/>
-      <c r="AD207" s="3"/>
-    </row>
-    <row r="208" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="208" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A208" s="21"/>
       <c r="B208" s="1"/>
       <c r="C208" s="3"/>
@@ -9094,9 +8847,8 @@
       <c r="AA208" s="3"/>
       <c r="AB208" s="3"/>
       <c r="AC208" s="26"/>
-      <c r="AD208" s="3"/>
-    </row>
-    <row r="209" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="209" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A209" s="20"/>
       <c r="B209" s="1"/>
       <c r="C209" s="1"/>
@@ -9126,9 +8878,8 @@
       <c r="AA209" s="1"/>
       <c r="AB209" s="1"/>
       <c r="AC209" s="25"/>
-      <c r="AD209" s="3"/>
-    </row>
-    <row r="210" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="210" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A210" s="21"/>
       <c r="B210" s="1"/>
       <c r="C210" s="3"/>
@@ -9158,9 +8909,8 @@
       <c r="AA210" s="3"/>
       <c r="AB210" s="3"/>
       <c r="AC210" s="26"/>
-      <c r="AD210" s="3"/>
-    </row>
-    <row r="211" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="211" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A211" s="20"/>
       <c r="B211" s="1"/>
       <c r="C211" s="1"/>
@@ -9190,9 +8940,8 @@
       <c r="AA211" s="1"/>
       <c r="AB211" s="1"/>
       <c r="AC211" s="25"/>
-      <c r="AD211" s="3"/>
-    </row>
-    <row r="212" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="212" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A212" s="21"/>
       <c r="B212" s="1"/>
       <c r="C212" s="3"/>
@@ -9222,9 +8971,8 @@
       <c r="AA212" s="3"/>
       <c r="AB212" s="3"/>
       <c r="AC212" s="26"/>
-      <c r="AD212" s="3"/>
-    </row>
-    <row r="213" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="213" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A213" s="20"/>
       <c r="B213" s="1"/>
       <c r="C213" s="1"/>
@@ -9254,9 +9002,8 @@
       <c r="AA213" s="1"/>
       <c r="AB213" s="1"/>
       <c r="AC213" s="25"/>
-      <c r="AD213" s="3"/>
-    </row>
-    <row r="214" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="214" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A214" s="21"/>
       <c r="B214" s="1"/>
       <c r="C214" s="1"/>
@@ -9286,9 +9033,8 @@
       <c r="AA214" s="3"/>
       <c r="AB214" s="3"/>
       <c r="AC214" s="26"/>
-      <c r="AD214" s="3"/>
-    </row>
-    <row r="215" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="215" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A215" s="20"/>
       <c r="B215" s="1"/>
       <c r="C215" s="1"/>
@@ -9318,9 +9064,8 @@
       <c r="AA215" s="1"/>
       <c r="AB215" s="1"/>
       <c r="AC215" s="25"/>
-      <c r="AD215" s="3"/>
-    </row>
-    <row r="216" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="216" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A216" s="21"/>
       <c r="B216" s="1"/>
       <c r="C216" s="1"/>
@@ -9350,9 +9095,8 @@
       <c r="AA216" s="3"/>
       <c r="AB216" s="3"/>
       <c r="AC216" s="26"/>
-      <c r="AD216" s="3"/>
-    </row>
-    <row r="217" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="217" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A217" s="20"/>
       <c r="B217" s="1"/>
       <c r="C217" s="1"/>
@@ -9382,9 +9126,8 @@
       <c r="AA217" s="1"/>
       <c r="AB217" s="1"/>
       <c r="AC217" s="25"/>
-      <c r="AD217" s="3"/>
-    </row>
-    <row r="218" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="218" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A218" s="21"/>
       <c r="B218" s="1"/>
       <c r="C218" s="1"/>
@@ -9414,9 +9157,8 @@
       <c r="AA218" s="3"/>
       <c r="AB218" s="3"/>
       <c r="AC218" s="26"/>
-      <c r="AD218" s="3"/>
-    </row>
-    <row r="219" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="219" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A219" s="20"/>
       <c r="B219" s="1"/>
       <c r="C219" s="1"/>
@@ -9446,9 +9188,8 @@
       <c r="AA219" s="1"/>
       <c r="AB219" s="1"/>
       <c r="AC219" s="25"/>
-      <c r="AD219" s="3"/>
-    </row>
-    <row r="220" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="220" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A220" s="21"/>
       <c r="B220" s="1"/>
       <c r="C220" s="3"/>
@@ -9478,9 +9219,8 @@
       <c r="AA220" s="3"/>
       <c r="AB220" s="3"/>
       <c r="AC220" s="26"/>
-      <c r="AD220" s="3"/>
-    </row>
-    <row r="221" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="221" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A221" s="20"/>
       <c r="B221" s="1"/>
       <c r="C221" s="1"/>
@@ -9510,9 +9250,8 @@
       <c r="AA221" s="1"/>
       <c r="AB221" s="1"/>
       <c r="AC221" s="25"/>
-      <c r="AD221" s="3"/>
-    </row>
-    <row r="222" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="222" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A222" s="21"/>
       <c r="B222" s="1"/>
       <c r="C222" s="1"/>
@@ -9542,9 +9281,8 @@
       <c r="AA222" s="3"/>
       <c r="AB222" s="3"/>
       <c r="AC222" s="26"/>
-      <c r="AD222" s="3"/>
-    </row>
-    <row r="223" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="223" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A223" s="20"/>
       <c r="B223" s="1"/>
       <c r="C223" s="1"/>
@@ -9574,9 +9312,8 @@
       <c r="AA223" s="1"/>
       <c r="AB223" s="1"/>
       <c r="AC223" s="25"/>
-      <c r="AD223" s="3"/>
-    </row>
-    <row r="224" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="224" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A224" s="21"/>
       <c r="B224" s="1"/>
       <c r="C224" s="1"/>
@@ -9606,9 +9343,8 @@
       <c r="AA224" s="3"/>
       <c r="AB224" s="3"/>
       <c r="AC224" s="26"/>
-      <c r="AD224" s="3"/>
-    </row>
-    <row r="225" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="225" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A225" s="20"/>
       <c r="B225" s="1"/>
       <c r="C225" s="1"/>
@@ -9638,9 +9374,8 @@
       <c r="AA225" s="1"/>
       <c r="AB225" s="1"/>
       <c r="AC225" s="25"/>
-      <c r="AD225" s="3"/>
-    </row>
-    <row r="226" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="226" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A226" s="21"/>
       <c r="B226" s="1"/>
       <c r="C226" s="1"/>
@@ -9670,9 +9405,8 @@
       <c r="AA226" s="3"/>
       <c r="AB226" s="3"/>
       <c r="AC226" s="26"/>
-      <c r="AD226" s="3"/>
-    </row>
-    <row r="227" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="227" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A227" s="20"/>
       <c r="B227" s="1"/>
       <c r="C227" s="1"/>
@@ -9702,9 +9436,8 @@
       <c r="AA227" s="1"/>
       <c r="AB227" s="1"/>
       <c r="AC227" s="25"/>
-      <c r="AD227" s="3"/>
-    </row>
-    <row r="228" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="228" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A228" s="21"/>
       <c r="B228" s="1"/>
       <c r="C228" s="1"/>
@@ -9734,9 +9467,8 @@
       <c r="AA228" s="3"/>
       <c r="AB228" s="3"/>
       <c r="AC228" s="26"/>
-      <c r="AD228" s="3"/>
-    </row>
-    <row r="229" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="229" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A229" s="20"/>
       <c r="B229" s="1"/>
       <c r="C229" s="1"/>
@@ -9766,9 +9498,8 @@
       <c r="AA229" s="1"/>
       <c r="AB229" s="1"/>
       <c r="AC229" s="25"/>
-      <c r="AD229" s="3"/>
-    </row>
-    <row r="230" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="230" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A230" s="21"/>
       <c r="B230" s="1"/>
       <c r="C230" s="1"/>
@@ -9798,9 +9529,8 @@
       <c r="AA230" s="3"/>
       <c r="AB230" s="3"/>
       <c r="AC230" s="26"/>
-      <c r="AD230" s="3"/>
-    </row>
-    <row r="231" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="231" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A231" s="20"/>
       <c r="B231" s="1"/>
       <c r="C231" s="1"/>
@@ -9830,9 +9560,8 @@
       <c r="AA231" s="1"/>
       <c r="AB231" s="1"/>
       <c r="AC231" s="25"/>
-      <c r="AD231" s="3"/>
-    </row>
-    <row r="232" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="232" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A232" s="21"/>
       <c r="B232" s="1"/>
       <c r="C232" s="1"/>
@@ -9862,9 +9591,8 @@
       <c r="AA232" s="3"/>
       <c r="AB232" s="3"/>
       <c r="AC232" s="26"/>
-      <c r="AD232" s="3"/>
-    </row>
-    <row r="233" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="233" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A233" s="20"/>
       <c r="B233" s="1"/>
       <c r="C233" s="1"/>
@@ -9894,9 +9622,8 @@
       <c r="AA233" s="1"/>
       <c r="AB233" s="1"/>
       <c r="AC233" s="25"/>
-      <c r="AD233" s="3"/>
-    </row>
-    <row r="234" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="234" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A234" s="21"/>
       <c r="B234" s="1"/>
       <c r="C234" s="1"/>
@@ -9926,9 +9653,8 @@
       <c r="AA234" s="3"/>
       <c r="AB234" s="3"/>
       <c r="AC234" s="26"/>
-      <c r="AD234" s="3"/>
-    </row>
-    <row r="235" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="235" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A235" s="20"/>
       <c r="B235" s="1"/>
       <c r="C235" s="1"/>
@@ -9958,9 +9684,8 @@
       <c r="AA235" s="1"/>
       <c r="AB235" s="1"/>
       <c r="AC235" s="25"/>
-      <c r="AD235" s="3"/>
-    </row>
-    <row r="236" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="236" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A236" s="21"/>
       <c r="B236" s="1"/>
       <c r="C236" s="1"/>
@@ -9990,9 +9715,8 @@
       <c r="AA236" s="3"/>
       <c r="AB236" s="3"/>
       <c r="AC236" s="26"/>
-      <c r="AD236" s="3"/>
-    </row>
-    <row r="237" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="237" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A237" s="20"/>
       <c r="B237" s="1"/>
       <c r="C237" s="1"/>
@@ -10022,9 +9746,8 @@
       <c r="AA237" s="1"/>
       <c r="AB237" s="1"/>
       <c r="AC237" s="25"/>
-      <c r="AD237" s="3"/>
-    </row>
-    <row r="238" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="238" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A238" s="21"/>
       <c r="B238" s="1"/>
       <c r="C238" s="1"/>
@@ -10054,9 +9777,8 @@
       <c r="AA238" s="3"/>
       <c r="AB238" s="3"/>
       <c r="AC238" s="26"/>
-      <c r="AD238" s="3"/>
-    </row>
-    <row r="239" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="239" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A239" s="20"/>
       <c r="B239" s="1"/>
       <c r="C239" s="1"/>
@@ -10086,9 +9808,8 @@
       <c r="AA239" s="1"/>
       <c r="AB239" s="1"/>
       <c r="AC239" s="25"/>
-      <c r="AD239" s="3"/>
-    </row>
-    <row r="240" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="240" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A240" s="21"/>
       <c r="B240" s="3"/>
       <c r="C240" s="3"/>
@@ -10118,9 +9839,8 @@
       <c r="AA240" s="3"/>
       <c r="AB240" s="3"/>
       <c r="AC240" s="26"/>
-      <c r="AD240" s="3"/>
-    </row>
-    <row r="241" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="241" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A241" s="20"/>
       <c r="B241" s="1"/>
       <c r="C241" s="1"/>
@@ -10150,9 +9870,8 @@
       <c r="AA241" s="1"/>
       <c r="AB241" s="1"/>
       <c r="AC241" s="25"/>
-      <c r="AD241" s="3"/>
-    </row>
-    <row r="242" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="242" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A242" s="21"/>
       <c r="B242" s="3"/>
       <c r="C242" s="3"/>
@@ -10182,9 +9901,8 @@
       <c r="AA242" s="3"/>
       <c r="AB242" s="3"/>
       <c r="AC242" s="26"/>
-      <c r="AD242" s="3"/>
-    </row>
-    <row r="243" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="243" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A243" s="20"/>
       <c r="B243" s="1"/>
       <c r="C243" s="1"/>
@@ -10214,9 +9932,8 @@
       <c r="AA243" s="1"/>
       <c r="AB243" s="1"/>
       <c r="AC243" s="25"/>
-      <c r="AD243" s="3"/>
-    </row>
-    <row r="244" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="244" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A244" s="21"/>
       <c r="B244" s="3"/>
       <c r="C244" s="3"/>
@@ -10246,9 +9963,8 @@
       <c r="AA244" s="3"/>
       <c r="AB244" s="3"/>
       <c r="AC244" s="26"/>
-      <c r="AD244" s="3"/>
-    </row>
-    <row r="245" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="245" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A245" s="20"/>
       <c r="B245" s="1"/>
       <c r="C245" s="1"/>
@@ -10278,9 +9994,8 @@
       <c r="AA245" s="1"/>
       <c r="AB245" s="1"/>
       <c r="AC245" s="25"/>
-      <c r="AD245" s="3"/>
-    </row>
-    <row r="246" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="246" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A246" s="21"/>
       <c r="B246" s="3"/>
       <c r="C246" s="3"/>
@@ -10310,9 +10025,8 @@
       <c r="AA246" s="3"/>
       <c r="AB246" s="3"/>
       <c r="AC246" s="26"/>
-      <c r="AD246" s="3"/>
-    </row>
-    <row r="247" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="247" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A247" s="20"/>
       <c r="B247" s="1"/>
       <c r="C247" s="1"/>
@@ -10342,9 +10056,8 @@
       <c r="AA247" s="1"/>
       <c r="AB247" s="1"/>
       <c r="AC247" s="25"/>
-      <c r="AD247" s="3"/>
-    </row>
-    <row r="248" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="248" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A248" s="21"/>
       <c r="B248" s="3"/>
       <c r="C248" s="3"/>
@@ -10374,9 +10087,8 @@
       <c r="AA248" s="3"/>
       <c r="AB248" s="3"/>
       <c r="AC248" s="26"/>
-      <c r="AD248" s="3"/>
-    </row>
-    <row r="249" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="249" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A249" s="20"/>
       <c r="B249" s="1"/>
       <c r="C249" s="1"/>
@@ -10406,9 +10118,8 @@
       <c r="AA249" s="1"/>
       <c r="AB249" s="1"/>
       <c r="AC249" s="25"/>
-      <c r="AD249" s="3"/>
-    </row>
-    <row r="250" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="250" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A250" s="21"/>
       <c r="B250" s="3"/>
       <c r="C250" s="3"/>
@@ -10438,9 +10149,8 @@
       <c r="AA250" s="3"/>
       <c r="AB250" s="3"/>
       <c r="AC250" s="26"/>
-      <c r="AD250" s="3"/>
-    </row>
-    <row r="251" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="251" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A251" s="20"/>
       <c r="B251" s="1"/>
       <c r="C251" s="1"/>
@@ -10470,9 +10180,8 @@
       <c r="AA251" s="1"/>
       <c r="AB251" s="1"/>
       <c r="AC251" s="25"/>
-      <c r="AD251" s="3"/>
-    </row>
-    <row r="252" spans="1:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="252" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A252" s="29"/>
       <c r="B252" s="30"/>
       <c r="C252" s="30"/>
@@ -10502,12 +10211,12 @@
       <c r="AA252" s="30"/>
       <c r="AB252" s="30"/>
       <c r="AC252" s="31"/>
-      <c r="AD252" s="30"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -10522,17 +10231,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="42" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="42" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="42" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deleting files/data not needed
</commit_message>
<xml_diff>
--- a/Data/Example_DB.xlsx
+++ b/Data/Example_DB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jones\Documents\CS_495\Group1_Project_Middle-Backend\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F10C7DB-5D7F-441B-94AA-12CD224BC8D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DB2FC26-226D-40AB-A60C-47D1EE29FA25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11832" yWindow="5220" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Project Name</t>
   </si>
@@ -38,9 +38,6 @@
   </si>
   <si>
     <t>Class Level</t>
-  </si>
-  <si>
-    <t>Course</t>
   </si>
   <si>
     <t>Primary Focus Area</t>
@@ -83,60 +80,6 @@
   </si>
   <si>
     <t>Admission Type</t>
-  </si>
-  <si>
-    <t>Anthropology is Elemental</t>
-  </si>
-  <si>
-    <t>Arts &amp; Science</t>
-  </si>
-  <si>
-    <t>Anthropology</t>
-  </si>
-  <si>
-    <t>400, 500</t>
-  </si>
-  <si>
-    <t>Community Education</t>
-  </si>
-  <si>
-    <t>Spring</t>
-  </si>
-  <si>
-    <t>Complete</t>
-  </si>
-  <si>
-    <t>Unpaid</t>
-  </si>
-  <si>
-    <t>Dr. Christopher Lynn</t>
-  </si>
-  <si>
-    <t>My Project</t>
-  </si>
-  <si>
-    <t>Engineering</t>
-  </si>
-  <si>
-    <t>Computer Science</t>
-  </si>
-  <si>
-    <t>400</t>
-  </si>
-  <si>
-    <t>10/03/2022</t>
-  </si>
-  <si>
-    <t>11/03/2022</t>
-  </si>
-  <si>
-    <t>Spring 2022</t>
-  </si>
-  <si>
-    <t>Active</t>
-  </si>
-  <si>
-    <t>Partner</t>
   </si>
   <si>
     <t>jnIAKtDwtECk6M5DPz-8p-dVhWE2MPxOupkWyXoPG15UNlJVSzBKREVTVVQ4VkI1SFo5TjMwOExYUC4u</t>
@@ -1120,20 +1063,16 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
         <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
-        <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="10"/>
         <color theme="1"/>
         <name val="Arial"/>
         <charset val="1"/>
-        <scheme val="none"/>
       </font>
       <fill>
         <patternFill patternType="solid">
@@ -1141,8 +1080,119 @@
           <bgColor rgb="FFF3F3F3"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <alignment horizontal="general" vertical="bottom" readingOrder="1"/>
+      <border>
+        <left style="thin">
+          <color rgb="FFCCCCCC"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFCCCCCC"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFCCCCCC"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FFCCCCCC"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <charset val="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFF3F3F3"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" readingOrder="1"/>
+      <border>
+        <left style="thin">
+          <color rgb="FFCCCCCC"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFCCCCCC"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFCCCCCC"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FFCCCCCC"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <charset val="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFF3F3F3"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" readingOrder="1"/>
+      <border>
+        <left style="thin">
+          <color rgb="FFCCCCCC"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFCCCCCC"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFCCCCCC"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FFCCCCCC"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <charset val="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFF3F3F3"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" readingOrder="1"/>
+      <border>
         <left style="thin">
           <color rgb="FFCCCCCC"/>
         </left>
@@ -1202,20 +1252,16 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
         <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
-        <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="10"/>
         <color theme="1"/>
         <name val="Arial"/>
         <charset val="1"/>
-        <scheme val="none"/>
       </font>
       <fill>
         <patternFill patternType="solid">
@@ -1223,8 +1269,8 @@
           <bgColor rgb="FFF3F3F3"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <alignment horizontal="general" vertical="bottom" readingOrder="1"/>
+      <border>
         <left style="thin">
           <color rgb="FFCCCCCC"/>
         </left>
@@ -1317,16 +1363,20 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
         <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
+        <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="10"/>
         <color theme="1"/>
         <name val="Arial"/>
         <charset val="1"/>
+        <scheme val="none"/>
       </font>
       <fill>
         <patternFill patternType="solid">
@@ -1334,8 +1384,8 @@
           <bgColor rgb="FFF3F3F3"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" vertical="bottom" readingOrder="1"/>
-      <border>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color rgb="FFCCCCCC"/>
         </left>
@@ -1354,16 +1404,20 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
         <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
+        <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="10"/>
         <color theme="1"/>
         <name val="Arial"/>
         <charset val="1"/>
+        <scheme val="none"/>
       </font>
       <fill>
         <patternFill patternType="solid">
@@ -1371,119 +1425,8 @@
           <bgColor rgb="FFF3F3F3"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" vertical="bottom" readingOrder="1"/>
-      <border>
-        <left style="thin">
-          <color rgb="FFCCCCCC"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFCCCCCC"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFCCCCCC"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FFCCCCCC"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <charset val="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFF3F3F3"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" readingOrder="1"/>
-      <border>
-        <left style="thin">
-          <color rgb="FFCCCCCC"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFCCCCCC"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFCCCCCC"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FFCCCCCC"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <charset val="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFF3F3F3"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" readingOrder="1"/>
-      <border>
-        <left style="thin">
-          <color rgb="FFCCCCCC"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFCCCCCC"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFCCCCCC"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FFCCCCCC"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <charset val="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFF3F3F3"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" readingOrder="1"/>
-      <border>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="1"/>
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color rgb="FFCCCCCC"/>
         </left>
@@ -1792,32 +1735,32 @@
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Department" dataDxfId="28"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Class Level" dataDxfId="27"/>
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Primary Focus Area" dataDxfId="26"/>
-    <tableColumn id="6" xr3:uid="{9B432CE0-DC0C-4BA7-AA64-BA3E966D0BEA}" name="Participant Type" dataDxfId="18"/>
-    <tableColumn id="7" xr3:uid="{59E89773-8224-4C13-B11F-867EFFBF47CC}" name="Number of Participants" dataDxfId="17"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Start Date" dataDxfId="25"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="End Date" dataDxfId="24"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Semester" dataDxfId="23"/>
-    <tableColumn id="30" xr3:uid="{6C19913E-0858-49D4-B470-82245D67396F}" name="Year" dataDxfId="16"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Status" dataDxfId="22"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Compensation" dataDxfId="21"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Opportunity Type" dataDxfId="20"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="University Partner" dataDxfId="19"/>
+    <tableColumn id="6" xr3:uid="{9B432CE0-DC0C-4BA7-AA64-BA3E966D0BEA}" name="Participant Type" dataDxfId="25"/>
+    <tableColumn id="7" xr3:uid="{59E89773-8224-4C13-B11F-867EFFBF47CC}" name="Number of Participants" dataDxfId="24"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Start Date" dataDxfId="23"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="End Date" dataDxfId="22"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Semester" dataDxfId="21"/>
+    <tableColumn id="30" xr3:uid="{6C19913E-0858-49D4-B470-82245D67396F}" name="Year" dataDxfId="20"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Status" dataDxfId="19"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Compensation" dataDxfId="18"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Opportunity Type" dataDxfId="17"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="University Partner" dataDxfId="16"/>
     <tableColumn id="31" xr3:uid="{B0DC1DBE-530B-411A-8617-4C43641D354F}" name="Working with a community partner?" dataDxfId="15"/>
-    <tableColumn id="33" xr3:uid="{B3D9DC91-615D-4D73-A835-462EF4A40ECD}" name="Association" dataDxfId="13"/>
-    <tableColumn id="34" xr3:uid="{BCA9E0AD-268A-47CE-A854-ECB3A0606165}" name="Type" dataDxfId="12"/>
-    <tableColumn id="35" xr3:uid="{752EA247-E69A-471D-BE04-0A2FFDF77C1F}" name="Contact" dataDxfId="11"/>
-    <tableColumn id="36" xr3:uid="{949CB3DF-FCFC-46FB-BDBF-BFC4B1E9A4B0}" name="Website" dataDxfId="10"/>
-    <tableColumn id="37" xr3:uid="{A579538F-A4F4-460D-A04B-CA4FE8CAA81E}" name="Address" dataDxfId="9"/>
-    <tableColumn id="38" xr3:uid="{1D993010-C598-4E80-BA95-AFF2E8D592DA}" name="Mode" dataDxfId="8"/>
-    <tableColumn id="39" xr3:uid="{248A0496-961C-4C4D-94F6-645645EEB666}" name="Financing" dataDxfId="7"/>
-    <tableColumn id="40" xr3:uid="{956953DD-876A-4CA2-9DAE-C6624FE66C0E}" name="Cost to Student" dataDxfId="6"/>
-    <tableColumn id="41" xr3:uid="{71E1DBD2-5111-41D7-87A3-2EBD0A831344}" name="Cost to UA Partner" dataDxfId="5"/>
-    <tableColumn id="42" xr3:uid="{4D7A91A1-8314-4D09-BCB9-565FC7840176}" name="Cost to Community Partner" dataDxfId="4"/>
-    <tableColumn id="43" xr3:uid="{84474C13-5D33-41A0-833C-171C7F3B7204}" name="Time Commitment" dataDxfId="3"/>
-    <tableColumn id="44" xr3:uid="{103C08F9-9301-44CA-9115-F0041251E65A}" name="Admission Type" dataDxfId="2"/>
-    <tableColumn id="45" xr3:uid="{AB7C5DBF-D8FF-49F4-AD7D-1D28EA4785AE}" name="Impact" dataDxfId="1"/>
-    <tableColumn id="46" xr3:uid="{F1142474-FB91-4DB2-8426-B34DB3DE835E}" name="Outreach" dataDxfId="0"/>
-    <tableColumn id="32" xr3:uid="{BD50DC1E-6155-48DF-AE14-8AE64E413B23}" name="Project Description" dataDxfId="14"/>
+    <tableColumn id="33" xr3:uid="{B3D9DC91-615D-4D73-A835-462EF4A40ECD}" name="Association" dataDxfId="14"/>
+    <tableColumn id="34" xr3:uid="{BCA9E0AD-268A-47CE-A854-ECB3A0606165}" name="Type" dataDxfId="13"/>
+    <tableColumn id="35" xr3:uid="{752EA247-E69A-471D-BE04-0A2FFDF77C1F}" name="Contact" dataDxfId="12"/>
+    <tableColumn id="36" xr3:uid="{949CB3DF-FCFC-46FB-BDBF-BFC4B1E9A4B0}" name="Website" dataDxfId="11"/>
+    <tableColumn id="37" xr3:uid="{A579538F-A4F4-460D-A04B-CA4FE8CAA81E}" name="Address" dataDxfId="10"/>
+    <tableColumn id="38" xr3:uid="{1D993010-C598-4E80-BA95-AFF2E8D592DA}" name="Mode" dataDxfId="9"/>
+    <tableColumn id="39" xr3:uid="{248A0496-961C-4C4D-94F6-645645EEB666}" name="Financing" dataDxfId="8"/>
+    <tableColumn id="40" xr3:uid="{956953DD-876A-4CA2-9DAE-C6624FE66C0E}" name="Cost to Student" dataDxfId="7"/>
+    <tableColumn id="41" xr3:uid="{71E1DBD2-5111-41D7-87A3-2EBD0A831344}" name="Cost to UA Partner" dataDxfId="6"/>
+    <tableColumn id="42" xr3:uid="{4D7A91A1-8314-4D09-BCB9-565FC7840176}" name="Cost to Community Partner" dataDxfId="5"/>
+    <tableColumn id="43" xr3:uid="{84474C13-5D33-41A0-833C-171C7F3B7204}" name="Time Commitment" dataDxfId="4"/>
+    <tableColumn id="44" xr3:uid="{103C08F9-9301-44CA-9115-F0041251E65A}" name="Admission Type" dataDxfId="3"/>
+    <tableColumn id="45" xr3:uid="{AB7C5DBF-D8FF-49F4-AD7D-1D28EA4785AE}" name="Impact" dataDxfId="2"/>
+    <tableColumn id="46" xr3:uid="{F1142474-FB91-4DB2-8426-B34DB3DE835E}" name="Outreach" dataDxfId="1"/>
+    <tableColumn id="32" xr3:uid="{BD50DC1E-6155-48DF-AE14-8AE64E413B23}" name="Project Description" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2123,17 +2066,18 @@
   <dimension ref="A1:AE252"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AE1" sqref="AE1"/>
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="41.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="41.88671875" customWidth="1"/>
+    <col min="5" max="5" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.88671875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17.88671875" bestFit="1" customWidth="1"/>
@@ -2141,13 +2085,21 @@
     <col min="12" max="12" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="32.88671875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="19.33203125" customWidth="1"/>
-    <col min="15" max="15" width="44.109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="23" width="44.109375" customWidth="1"/>
+    <col min="15" max="15" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="34.109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.21875" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="18.88671875" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="18.88671875" customWidth="1"/>
     <col min="27" max="27" width="19" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="9.109375" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="11" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="19.21875" bestFit="1" customWidth="1"/>
   </cols>
@@ -2166,127 +2118,103 @@
         <v>3</v>
       </c>
       <c r="E1" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="26" t="s">
-        <v>40</v>
+      <c r="I1" s="18" t="s">
+        <v>6</v>
       </c>
-      <c r="G1" s="26" t="s">
+      <c r="J1" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="O1" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="P1" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q1" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="R1" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="S1" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="T1" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="U1" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="V1" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="18" t="s">
-        <v>6</v>
+      <c r="W1" s="27" t="s">
+        <v>29</v>
       </c>
-      <c r="I1" s="18" t="s">
+      <c r="X1" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="Y1" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="Z1" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA1" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB1" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="AC1" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="AD1" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="AE1" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="26" t="s">
-        <v>41</v>
-      </c>
-      <c r="L1" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q1" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="R1" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="S1" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="T1" s="27" t="s">
-        <v>46</v>
-      </c>
-      <c r="U1" s="27" t="s">
-        <v>47</v>
-      </c>
-      <c r="V1" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="W1" s="27" t="s">
-        <v>48</v>
-      </c>
-      <c r="X1" s="27" t="s">
-        <v>49</v>
-      </c>
-      <c r="Y1" s="27" t="s">
-        <v>50</v>
-      </c>
-      <c r="Z1" s="27" t="s">
-        <v>51</v>
-      </c>
-      <c r="AA1" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="AB1" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="AC1" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="AD1" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="AE1" s="27" t="s">
-        <v>8</v>
-      </c>
     </row>
     <row r="2" spans="1:31" ht="53.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>23</v>
-      </c>
+      <c r="A2" s="11"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
-      <c r="H2" s="1">
-        <v>2019</v>
-      </c>
-      <c r="I2" s="1">
-        <v>2019</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
       <c r="K2" s="1"/>
-      <c r="L2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>27</v>
-      </c>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
       <c r="P2" s="1"/>
       <c r="Q2" s="16"/>
       <c r="R2" s="16"/>
@@ -2305,45 +2233,21 @@
       <c r="AE2" s="16"/>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A3" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>29</v>
-      </c>
+      <c r="A3" s="12"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
-      <c r="H3" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>34</v>
-      </c>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
       <c r="K3" s="2"/>
-      <c r="L3" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>36</v>
-      </c>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
       <c r="P3" s="2"/>
       <c r="Q3" s="17"/>
       <c r="R3" s="17"/>
@@ -10597,17 +10501,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="24" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="24" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated excel file. Removed hardcoded field array
</commit_message>
<xml_diff>
--- a/Data/Example_DB.xlsx
+++ b/Data/Example_DB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jones\Documents\CS_495\Group1_Project_Middle-Backend\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DB2FC26-226D-40AB-A60C-47D1EE29FA25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B4E3E84-BF6D-40C1-9719-42A50D60B4D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4728" yWindow="0" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,60 +28,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
-    <t>Project Name</t>
-  </si>
-  <si>
-    <t>College</t>
-  </si>
-  <si>
-    <t>Department</t>
-  </si>
-  <si>
-    <t>Class Level</t>
-  </si>
-  <si>
-    <t>Primary Focus Area</t>
-  </si>
-  <si>
-    <t>Start Date</t>
-  </si>
-  <si>
-    <t>End Date</t>
-  </si>
-  <si>
-    <t>Project Description</t>
-  </si>
-  <si>
-    <t>Semester</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>Compensation</t>
-  </si>
-  <si>
-    <t>Opportunity Type</t>
-  </si>
-  <si>
-    <t>University Partner</t>
-  </si>
-  <si>
-    <t>Number of Participants</t>
-  </si>
-  <si>
-    <t>Mode</t>
-  </si>
-  <si>
-    <t>Impact</t>
-  </si>
-  <si>
-    <t>Time Commitment</t>
-  </si>
-  <si>
-    <t>Admission Type</t>
-  </si>
-  <si>
     <t>jnIAKtDwtECk6M5DPz-8p-dVhWE2MPxOupkWyXoPG15UNlJVSzBKREVTVVQ4VkI1SFo5TjMwOExYUC4u</t>
   </si>
   <si>
@@ -91,63 +37,110 @@
     <t>{439e710e-9363-46fe-b6b8-d105e96ee7e6}</t>
   </si>
   <si>
-    <t>Participant Type</t>
+    <t>project_name</t>
   </si>
   <si>
-    <t>Year</t>
+    <t>college</t>
   </si>
   <si>
-    <t>Working with a community partner?</t>
+    <t>department</t>
   </si>
   <si>
-    <t>Association</t>
+    <t>class_level</t>
   </si>
   <si>
-    <t>Type</t>
+    <t>primary_focus_area</t>
   </si>
   <si>
-    <t>Contact</t>
+    <t>participant_type</t>
   </si>
   <si>
-    <t>Website</t>
+    <t>number_of_participants</t>
   </si>
   <si>
-    <t>Address</t>
+    <t>start_date</t>
   </si>
   <si>
-    <t>Financing</t>
+    <t>end_date</t>
   </si>
   <si>
-    <t>Cost to Student</t>
+    <t>semester</t>
   </si>
   <si>
-    <t>Cost to UA Partner</t>
+    <t>year</t>
   </si>
   <si>
-    <t>Cost to Community Partner</t>
+    <t>status</t>
   </si>
   <si>
-    <t>Outreach</t>
+    <t>compensation</t>
+  </si>
+  <si>
+    <t>association</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>contact</t>
+  </si>
+  <si>
+    <t>website</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>mode</t>
+  </si>
+  <si>
+    <t>financing</t>
+  </si>
+  <si>
+    <t>cost_to_student</t>
+  </si>
+  <si>
+    <t>cost_to_ua_partner</t>
+  </si>
+  <si>
+    <t>cost_to_community_partner</t>
+  </si>
+  <si>
+    <t>time_commitment</t>
+  </si>
+  <si>
+    <t>admission_type</t>
+  </si>
+  <si>
+    <t>impact</t>
+  </si>
+  <si>
+    <t>outreach</t>
+  </si>
+  <si>
+    <t>opportunity_type</t>
+  </si>
+  <si>
+    <t>university_partner</t>
+  </si>
+  <si>
+    <t>working_with_a_community_partner</t>
+  </si>
+  <si>
+    <t>description_1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -349,21 +342,30 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
     <xf numFmtId="14" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -372,62 +374,50 @@
     <xf numFmtId="14" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
-    <xf numFmtId="14" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -1730,37 +1720,37 @@
     </filterColumn>
   </autoFilter>
   <tableColumns count="31">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Project Name" dataDxfId="30"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="College" dataDxfId="29"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Department" dataDxfId="28"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Class Level" dataDxfId="27"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Primary Focus Area" dataDxfId="26"/>
-    <tableColumn id="6" xr3:uid="{9B432CE0-DC0C-4BA7-AA64-BA3E966D0BEA}" name="Participant Type" dataDxfId="25"/>
-    <tableColumn id="7" xr3:uid="{59E89773-8224-4C13-B11F-867EFFBF47CC}" name="Number of Participants" dataDxfId="24"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Start Date" dataDxfId="23"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="End Date" dataDxfId="22"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Semester" dataDxfId="21"/>
-    <tableColumn id="30" xr3:uid="{6C19913E-0858-49D4-B470-82245D67396F}" name="Year" dataDxfId="20"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Status" dataDxfId="19"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Compensation" dataDxfId="18"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Opportunity Type" dataDxfId="17"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="University Partner" dataDxfId="16"/>
-    <tableColumn id="31" xr3:uid="{B0DC1DBE-530B-411A-8617-4C43641D354F}" name="Working with a community partner?" dataDxfId="15"/>
-    <tableColumn id="33" xr3:uid="{B3D9DC91-615D-4D73-A835-462EF4A40ECD}" name="Association" dataDxfId="14"/>
-    <tableColumn id="34" xr3:uid="{BCA9E0AD-268A-47CE-A854-ECB3A0606165}" name="Type" dataDxfId="13"/>
-    <tableColumn id="35" xr3:uid="{752EA247-E69A-471D-BE04-0A2FFDF77C1F}" name="Contact" dataDxfId="12"/>
-    <tableColumn id="36" xr3:uid="{949CB3DF-FCFC-46FB-BDBF-BFC4B1E9A4B0}" name="Website" dataDxfId="11"/>
-    <tableColumn id="37" xr3:uid="{A579538F-A4F4-460D-A04B-CA4FE8CAA81E}" name="Address" dataDxfId="10"/>
-    <tableColumn id="38" xr3:uid="{1D993010-C598-4E80-BA95-AFF2E8D592DA}" name="Mode" dataDxfId="9"/>
-    <tableColumn id="39" xr3:uid="{248A0496-961C-4C4D-94F6-645645EEB666}" name="Financing" dataDxfId="8"/>
-    <tableColumn id="40" xr3:uid="{956953DD-876A-4CA2-9DAE-C6624FE66C0E}" name="Cost to Student" dataDxfId="7"/>
-    <tableColumn id="41" xr3:uid="{71E1DBD2-5111-41D7-87A3-2EBD0A831344}" name="Cost to UA Partner" dataDxfId="6"/>
-    <tableColumn id="42" xr3:uid="{4D7A91A1-8314-4D09-BCB9-565FC7840176}" name="Cost to Community Partner" dataDxfId="5"/>
-    <tableColumn id="43" xr3:uid="{84474C13-5D33-41A0-833C-171C7F3B7204}" name="Time Commitment" dataDxfId="4"/>
-    <tableColumn id="44" xr3:uid="{103C08F9-9301-44CA-9115-F0041251E65A}" name="Admission Type" dataDxfId="3"/>
-    <tableColumn id="45" xr3:uid="{AB7C5DBF-D8FF-49F4-AD7D-1D28EA4785AE}" name="Impact" dataDxfId="2"/>
-    <tableColumn id="46" xr3:uid="{F1142474-FB91-4DB2-8426-B34DB3DE835E}" name="Outreach" dataDxfId="1"/>
-    <tableColumn id="32" xr3:uid="{BD50DC1E-6155-48DF-AE14-8AE64E413B23}" name="Project Description" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="project_name" dataDxfId="30"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="college" dataDxfId="29"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="department" dataDxfId="28"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="class_level" dataDxfId="27"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="primary_focus_area" dataDxfId="26"/>
+    <tableColumn id="6" xr3:uid="{9B432CE0-DC0C-4BA7-AA64-BA3E966D0BEA}" name="participant_type" dataDxfId="25"/>
+    <tableColumn id="7" xr3:uid="{59E89773-8224-4C13-B11F-867EFFBF47CC}" name="number_of_participants" dataDxfId="24"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="start_date" dataDxfId="23"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="end_date" dataDxfId="22"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="semester" dataDxfId="21"/>
+    <tableColumn id="30" xr3:uid="{6C19913E-0858-49D4-B470-82245D67396F}" name="year" dataDxfId="20"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="status" dataDxfId="19"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="compensation" dataDxfId="18"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="opportunity_type" dataDxfId="17"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="university_partner" dataDxfId="16"/>
+    <tableColumn id="31" xr3:uid="{B0DC1DBE-530B-411A-8617-4C43641D354F}" name="working_with_a_community_partner" dataDxfId="15"/>
+    <tableColumn id="33" xr3:uid="{B3D9DC91-615D-4D73-A835-462EF4A40ECD}" name="association" dataDxfId="14"/>
+    <tableColumn id="34" xr3:uid="{BCA9E0AD-268A-47CE-A854-ECB3A0606165}" name="type" dataDxfId="13"/>
+    <tableColumn id="35" xr3:uid="{752EA247-E69A-471D-BE04-0A2FFDF77C1F}" name="contact" dataDxfId="12"/>
+    <tableColumn id="36" xr3:uid="{949CB3DF-FCFC-46FB-BDBF-BFC4B1E9A4B0}" name="website" dataDxfId="11"/>
+    <tableColumn id="37" xr3:uid="{A579538F-A4F4-460D-A04B-CA4FE8CAA81E}" name="address" dataDxfId="10"/>
+    <tableColumn id="38" xr3:uid="{1D993010-C598-4E80-BA95-AFF2E8D592DA}" name="mode" dataDxfId="9"/>
+    <tableColumn id="39" xr3:uid="{248A0496-961C-4C4D-94F6-645645EEB666}" name="financing" dataDxfId="8"/>
+    <tableColumn id="40" xr3:uid="{956953DD-876A-4CA2-9DAE-C6624FE66C0E}" name="cost_to_student" dataDxfId="7"/>
+    <tableColumn id="41" xr3:uid="{71E1DBD2-5111-41D7-87A3-2EBD0A831344}" name="cost_to_ua_partner" dataDxfId="6"/>
+    <tableColumn id="42" xr3:uid="{4D7A91A1-8314-4D09-BCB9-565FC7840176}" name="cost_to_community_partner" dataDxfId="5"/>
+    <tableColumn id="43" xr3:uid="{84474C13-5D33-41A0-833C-171C7F3B7204}" name="time_commitment" dataDxfId="4"/>
+    <tableColumn id="44" xr3:uid="{103C08F9-9301-44CA-9115-F0041251E65A}" name="admission_type" dataDxfId="3"/>
+    <tableColumn id="45" xr3:uid="{AB7C5DBF-D8FF-49F4-AD7D-1D28EA4785AE}" name="impact" dataDxfId="2"/>
+    <tableColumn id="46" xr3:uid="{F1142474-FB91-4DB2-8426-B34DB3DE835E}" name="outreach" dataDxfId="1"/>
+    <tableColumn id="32" xr3:uid="{BD50DC1E-6155-48DF-AE14-8AE64E413B23}" name="description_1" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2065,13 +2055,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE252"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+    <sheetView tabSelected="1" topLeftCell="AC1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AE1" sqref="AE1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
@@ -2086,7 +2076,7 @@
     <col min="13" max="13" width="32.88671875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="19.33203125" customWidth="1"/>
     <col min="15" max="15" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="34.109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="36.109375" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="12.77734375" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="7.33203125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="9.77734375" bestFit="1" customWidth="1"/>
@@ -2094,109 +2084,109 @@
     <col min="21" max="21" width="9.88671875" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="8.21875" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="18.88671875" customWidth="1"/>
+    <col min="24" max="24" width="17" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="20" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="27.77734375" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="19" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="16.5546875" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="9.109375" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="11" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="19.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A1" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="18" t="s">
+      <c r="A1" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="B1" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="C1" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="M1" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="N1" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="O1" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="P1" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q1" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="26" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="26" t="s">
+      <c r="W1" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="L1" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="M1" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="N1" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="O1" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="P1" s="26" t="s">
+      <c r="X1" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="Q1" s="27" t="s">
+      <c r="Y1" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="R1" s="27" t="s">
+      <c r="Z1" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="S1" s="27" t="s">
+      <c r="AA1" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="T1" s="27" t="s">
+      <c r="AB1" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="U1" s="27" t="s">
+      <c r="AC1" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="V1" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="W1" s="27" t="s">
+      <c r="AD1" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="X1" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="Y1" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="Z1" s="27" t="s">
-        <v>32</v>
-      </c>
-      <c r="AA1" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="AB1" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="AC1" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="AD1" s="27" t="s">
+      <c r="AE1" s="26" t="s">
         <v>33</v>
-      </c>
-      <c r="AE1" s="27" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:31" ht="53.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -5137,7 +5127,7 @@
       <c r="AE90" s="17"/>
     </row>
     <row r="91" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A91" s="23"/>
+      <c r="A91" s="22"/>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
       <c r="D91" s="1"/>
@@ -5170,7 +5160,7 @@
       <c r="AE91" s="16"/>
     </row>
     <row r="92" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A92" s="23"/>
+      <c r="A92" s="22"/>
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
       <c r="D92" s="2"/>
@@ -5203,7 +5193,7 @@
       <c r="AE92" s="17"/>
     </row>
     <row r="93" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A93" s="23"/>
+      <c r="A93" s="22"/>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
       <c r="D93" s="1"/>
@@ -5236,7 +5226,7 @@
       <c r="AE93" s="16"/>
     </row>
     <row r="94" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A94" s="23"/>
+      <c r="A94" s="22"/>
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
       <c r="D94" s="2"/>
@@ -5269,7 +5259,7 @@
       <c r="AE94" s="17"/>
     </row>
     <row r="95" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A95" s="23"/>
+      <c r="A95" s="22"/>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
       <c r="D95" s="1"/>
@@ -5302,7 +5292,7 @@
       <c r="AE95" s="16"/>
     </row>
     <row r="96" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A96" s="23"/>
+      <c r="A96" s="22"/>
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
       <c r="D96" s="2"/>
@@ -5335,7 +5325,7 @@
       <c r="AE96" s="17"/>
     </row>
     <row r="97" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A97" s="23"/>
+      <c r="A97" s="22"/>
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
       <c r="D97" s="2"/>
@@ -5368,7 +5358,7 @@
       <c r="AE97" s="17"/>
     </row>
     <row r="98" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A98" s="23"/>
+      <c r="A98" s="22"/>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
       <c r="D98" s="1"/>
@@ -5401,7 +5391,7 @@
       <c r="AE98" s="16"/>
     </row>
     <row r="99" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A99" s="23"/>
+      <c r="A99" s="22"/>
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
       <c r="D99" s="1"/>
@@ -5434,7 +5424,7 @@
       <c r="AE99" s="16"/>
     </row>
     <row r="100" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A100" s="22"/>
+      <c r="A100" s="21"/>
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
       <c r="D100" s="2"/>
@@ -5467,7 +5457,7 @@
       <c r="AE100" s="17"/>
     </row>
     <row r="101" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A101" s="22"/>
+      <c r="A101" s="21"/>
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
       <c r="D101" s="1"/>
@@ -5500,7 +5490,7 @@
       <c r="AE101" s="16"/>
     </row>
     <row r="102" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A102" s="22"/>
+      <c r="A102" s="21"/>
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
       <c r="D102" s="1"/>
@@ -10450,37 +10440,37 @@
       <c r="AE251" s="16"/>
     </row>
     <row r="252" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A252" s="19"/>
-      <c r="B252" s="20"/>
-      <c r="C252" s="20"/>
-      <c r="D252" s="20"/>
-      <c r="E252" s="20"/>
-      <c r="F252" s="20"/>
-      <c r="G252" s="20"/>
-      <c r="H252" s="20"/>
-      <c r="I252" s="20"/>
-      <c r="J252" s="20"/>
-      <c r="K252" s="20"/>
-      <c r="L252" s="20"/>
-      <c r="M252" s="20"/>
-      <c r="N252" s="20"/>
-      <c r="O252" s="20"/>
-      <c r="P252" s="20"/>
-      <c r="Q252" s="21"/>
-      <c r="R252" s="21"/>
-      <c r="S252" s="21"/>
-      <c r="T252" s="21"/>
-      <c r="U252" s="21"/>
-      <c r="V252" s="21"/>
-      <c r="W252" s="21"/>
-      <c r="X252" s="21"/>
-      <c r="Y252" s="21"/>
-      <c r="Z252" s="21"/>
-      <c r="AA252" s="21"/>
-      <c r="AB252" s="21"/>
-      <c r="AC252" s="21"/>
-      <c r="AD252" s="21"/>
-      <c r="AE252" s="21"/>
+      <c r="A252" s="18"/>
+      <c r="B252" s="19"/>
+      <c r="C252" s="19"/>
+      <c r="D252" s="19"/>
+      <c r="E252" s="19"/>
+      <c r="F252" s="19"/>
+      <c r="G252" s="19"/>
+      <c r="H252" s="19"/>
+      <c r="I252" s="19"/>
+      <c r="J252" s="19"/>
+      <c r="K252" s="19"/>
+      <c r="L252" s="19"/>
+      <c r="M252" s="19"/>
+      <c r="N252" s="19"/>
+      <c r="O252" s="19"/>
+      <c r="P252" s="19"/>
+      <c r="Q252" s="20"/>
+      <c r="R252" s="20"/>
+      <c r="S252" s="20"/>
+      <c r="T252" s="20"/>
+      <c r="U252" s="20"/>
+      <c r="V252" s="20"/>
+      <c r="W252" s="20"/>
+      <c r="X252" s="20"/>
+      <c r="Y252" s="20"/>
+      <c r="Z252" s="20"/>
+      <c r="AA252" s="20"/>
+      <c r="AB252" s="20"/>
+      <c r="AC252" s="20"/>
+      <c r="AD252" s="20"/>
+      <c r="AE252" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10500,18 +10490,18 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="24" t="s">
-        <v>18</v>
+      <c r="A1" s="23" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" s="24" t="s">
-        <v>19</v>
+      <c r="A2" s="23" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" s="24" t="s">
-        <v>20</v>
+      <c r="A3" s="23" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>